<commit_message>
Additional results and report
results for reduced, ngram and bigram fitness, version 0.1 report
</commit_message>
<xml_diff>
--- a/Documentation/Design/Cipher Models.xlsx
+++ b/Documentation/Design/Cipher Models.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="28755" windowHeight="12585" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="28755" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="Z340" sheetId="1" r:id="rId1"/>
@@ -386,8 +386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BN343"/>
   <sheetViews>
-    <sheetView topLeftCell="A306" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="K47" sqref="K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2240,196 +2240,1188 @@
         <v>29</v>
       </c>
       <c r="B30" s="2"/>
-      <c r="T30" s="1"/>
+      <c r="D30" s="2">
+        <v>1</v>
+      </c>
+      <c r="E30" s="2">
+        <v>2</v>
+      </c>
+      <c r="F30" s="2">
+        <v>3</v>
+      </c>
+      <c r="G30" s="2">
+        <v>4</v>
+      </c>
+      <c r="H30" s="2">
+        <v>5</v>
+      </c>
+      <c r="I30" s="2">
+        <v>6</v>
+      </c>
+      <c r="J30" s="2">
+        <v>7</v>
+      </c>
+      <c r="K30" s="2">
+        <v>8</v>
+      </c>
+      <c r="L30" s="2">
+        <v>9</v>
+      </c>
+      <c r="M30" s="2">
+        <v>10</v>
+      </c>
+      <c r="N30" s="2">
+        <v>11</v>
+      </c>
+      <c r="O30" s="2">
+        <v>12</v>
+      </c>
+      <c r="P30" s="2">
+        <v>13</v>
+      </c>
+      <c r="Q30" s="2">
+        <v>14</v>
+      </c>
+      <c r="R30" s="2">
+        <v>15</v>
+      </c>
+      <c r="S30" s="2">
+        <v>16</v>
+      </c>
+      <c r="T30" s="2">
+        <v>17</v>
+      </c>
     </row>
     <row r="31" spans="1:29" ht="15.75">
       <c r="A31" s="2">
         <v>30</v>
       </c>
       <c r="B31" s="2"/>
-      <c r="T31" s="1"/>
+      <c r="D31" s="2">
+        <v>18</v>
+      </c>
+      <c r="E31" s="2">
+        <v>5</v>
+      </c>
+      <c r="F31" s="2">
+        <v>19</v>
+      </c>
+      <c r="G31" s="2">
+        <v>20</v>
+      </c>
+      <c r="H31" s="2">
+        <v>21</v>
+      </c>
+      <c r="I31" s="2">
+        <v>22</v>
+      </c>
+      <c r="J31" s="2">
+        <v>23</v>
+      </c>
+      <c r="K31" s="2">
+        <v>24</v>
+      </c>
+      <c r="L31" s="2">
+        <v>25</v>
+      </c>
+      <c r="M31" s="2">
+        <v>26</v>
+      </c>
+      <c r="N31" s="2">
+        <v>27</v>
+      </c>
+      <c r="O31" s="2">
+        <v>28</v>
+      </c>
+      <c r="P31" s="2">
+        <v>29</v>
+      </c>
+      <c r="Q31" s="2">
+        <v>30</v>
+      </c>
+      <c r="R31" s="2">
+        <v>31</v>
+      </c>
+      <c r="S31" s="2">
+        <v>32</v>
+      </c>
+      <c r="T31" s="2">
+        <v>33</v>
+      </c>
     </row>
     <row r="32" spans="1:29" ht="15.75">
       <c r="A32" s="2">
         <v>31</v>
       </c>
       <c r="B32" s="2"/>
-      <c r="T32" s="1"/>
+      <c r="D32" s="2">
+        <v>20</v>
+      </c>
+      <c r="E32" s="2">
+        <v>34</v>
+      </c>
+      <c r="F32" s="2">
+        <v>35</v>
+      </c>
+      <c r="G32" s="2">
+        <v>36</v>
+      </c>
+      <c r="H32" s="2">
+        <v>37</v>
+      </c>
+      <c r="I32" s="2">
+        <v>19</v>
+      </c>
+      <c r="J32" s="2">
+        <v>38</v>
+      </c>
+      <c r="K32" s="2">
+        <v>39</v>
+      </c>
+      <c r="L32" s="2">
+        <v>15</v>
+      </c>
+      <c r="M32" s="2">
+        <v>26</v>
+      </c>
+      <c r="N32" s="2">
+        <v>21</v>
+      </c>
+      <c r="O32" s="2">
+        <v>33</v>
+      </c>
+      <c r="P32" s="2">
+        <v>13</v>
+      </c>
+      <c r="Q32" s="2">
+        <v>22</v>
+      </c>
+      <c r="R32" s="2">
+        <v>40</v>
+      </c>
+      <c r="S32" s="2">
+        <v>1</v>
+      </c>
+      <c r="T32" s="2">
+        <v>41</v>
+      </c>
     </row>
     <row r="33" spans="1:20" ht="15.75">
       <c r="A33" s="2">
         <v>32</v>
       </c>
       <c r="B33" s="2"/>
-      <c r="T33" s="1"/>
+      <c r="D33" s="2">
+        <v>42</v>
+      </c>
+      <c r="E33" s="2">
+        <v>5</v>
+      </c>
+      <c r="F33" s="2">
+        <v>5</v>
+      </c>
+      <c r="G33" s="2">
+        <v>43</v>
+      </c>
+      <c r="H33" s="2">
+        <v>7</v>
+      </c>
+      <c r="I33" s="2">
+        <v>6</v>
+      </c>
+      <c r="J33" s="2">
+        <v>44</v>
+      </c>
+      <c r="K33" s="2">
+        <v>30</v>
+      </c>
+      <c r="L33" s="2">
+        <v>8</v>
+      </c>
+      <c r="M33" s="2">
+        <v>45</v>
+      </c>
+      <c r="N33" s="2">
+        <v>5</v>
+      </c>
+      <c r="O33" s="2">
+        <v>23</v>
+      </c>
+      <c r="P33" s="2">
+        <v>19</v>
+      </c>
+      <c r="Q33" s="2">
+        <v>19</v>
+      </c>
+      <c r="R33" s="2">
+        <v>3</v>
+      </c>
+      <c r="S33" s="2">
+        <v>31</v>
+      </c>
+      <c r="T33" s="2">
+        <v>16</v>
+      </c>
     </row>
     <row r="34" spans="1:20" ht="15.75">
       <c r="A34" s="2">
         <v>33</v>
       </c>
       <c r="B34" s="2"/>
-      <c r="T34" s="1"/>
+      <c r="D34" s="2">
+        <v>46</v>
+      </c>
+      <c r="E34" s="2">
+        <v>47</v>
+      </c>
+      <c r="F34" s="2">
+        <v>37</v>
+      </c>
+      <c r="G34" s="2">
+        <v>19</v>
+      </c>
+      <c r="H34" s="2">
+        <v>40</v>
+      </c>
+      <c r="I34" s="2">
+        <v>48</v>
+      </c>
+      <c r="J34" s="2">
+        <v>49</v>
+      </c>
+      <c r="K34" s="2">
+        <v>17</v>
+      </c>
+      <c r="L34" s="2">
+        <v>11</v>
+      </c>
+      <c r="M34" s="2">
+        <v>50</v>
+      </c>
+      <c r="N34" s="2">
+        <v>51</v>
+      </c>
+      <c r="O34" s="2">
+        <v>9</v>
+      </c>
+      <c r="P34" s="2">
+        <v>19</v>
+      </c>
+      <c r="Q34" s="2">
+        <v>52</v>
+      </c>
+      <c r="R34" s="2">
+        <v>53</v>
+      </c>
+      <c r="S34" s="2">
+        <v>10</v>
+      </c>
+      <c r="T34" s="2">
+        <v>54</v>
+      </c>
     </row>
     <row r="35" spans="1:20" ht="15.75">
       <c r="A35" s="2">
         <v>20</v>
       </c>
       <c r="B35" s="2"/>
-      <c r="T35" s="1"/>
+      <c r="D35" s="2">
+        <v>5</v>
+      </c>
+      <c r="E35" s="2">
+        <v>44</v>
+      </c>
+      <c r="F35" s="2">
+        <v>3</v>
+      </c>
+      <c r="G35" s="2">
+        <v>7</v>
+      </c>
+      <c r="H35" s="2">
+        <v>51</v>
+      </c>
+      <c r="I35" s="2">
+        <v>6</v>
+      </c>
+      <c r="J35" s="2">
+        <v>23</v>
+      </c>
+      <c r="K35" s="2">
+        <v>55</v>
+      </c>
+      <c r="L35" s="2">
+        <v>30</v>
+      </c>
+      <c r="M35" s="2">
+        <v>17</v>
+      </c>
+      <c r="N35" s="2">
+        <v>56</v>
+      </c>
+      <c r="O35" s="2">
+        <v>10</v>
+      </c>
+      <c r="P35" s="2">
+        <v>51</v>
+      </c>
+      <c r="Q35" s="2">
+        <v>4</v>
+      </c>
+      <c r="R35" s="2">
+        <v>16</v>
+      </c>
+      <c r="S35" s="2">
+        <v>25</v>
+      </c>
+      <c r="T35" s="2">
+        <v>21</v>
+      </c>
     </row>
     <row r="36" spans="1:20" ht="15.75">
       <c r="A36" s="2">
         <v>34</v>
       </c>
       <c r="B36" s="2"/>
-      <c r="T36" s="1"/>
+      <c r="D36" s="2">
+        <v>22</v>
+      </c>
+      <c r="E36" s="2">
+        <v>50</v>
+      </c>
+      <c r="F36" s="2">
+        <v>19</v>
+      </c>
+      <c r="G36" s="2">
+        <v>31</v>
+      </c>
+      <c r="H36" s="2">
+        <v>57</v>
+      </c>
+      <c r="I36" s="2">
+        <v>24</v>
+      </c>
+      <c r="J36" s="2">
+        <v>58</v>
+      </c>
+      <c r="K36" s="2">
+        <v>16</v>
+      </c>
+      <c r="L36" s="2">
+        <v>38</v>
+      </c>
+      <c r="M36" s="2">
+        <v>36</v>
+      </c>
+      <c r="N36" s="2">
+        <v>59</v>
+      </c>
+      <c r="O36" s="2">
+        <v>15</v>
+      </c>
+      <c r="P36" s="2">
+        <v>8</v>
+      </c>
+      <c r="Q36" s="2">
+        <v>28</v>
+      </c>
+      <c r="R36" s="2">
+        <v>40</v>
+      </c>
+      <c r="S36" s="2">
+        <v>13</v>
+      </c>
+      <c r="T36" s="2">
+        <v>11</v>
+      </c>
     </row>
     <row r="37" spans="1:20" ht="15.75">
       <c r="A37" s="2">
         <v>35</v>
       </c>
       <c r="B37" s="2"/>
-      <c r="T37" s="1"/>
+      <c r="D37" s="2">
+        <v>21</v>
+      </c>
+      <c r="E37" s="2">
+        <v>15</v>
+      </c>
+      <c r="F37" s="2">
+        <v>16</v>
+      </c>
+      <c r="G37" s="2">
+        <v>41</v>
+      </c>
+      <c r="H37" s="2">
+        <v>32</v>
+      </c>
+      <c r="I37" s="2">
+        <v>49</v>
+      </c>
+      <c r="J37" s="2">
+        <v>22</v>
+      </c>
+      <c r="K37" s="2">
+        <v>23</v>
+      </c>
+      <c r="L37" s="2">
+        <v>19</v>
+      </c>
+      <c r="M37" s="2">
+        <v>46</v>
+      </c>
+      <c r="N37" s="2">
+        <v>18</v>
+      </c>
+      <c r="O37" s="2">
+        <v>27</v>
+      </c>
+      <c r="P37" s="2">
+        <v>40</v>
+      </c>
+      <c r="Q37" s="2">
+        <v>19</v>
+      </c>
+      <c r="R37" s="2">
+        <v>60</v>
+      </c>
+      <c r="S37" s="2">
+        <v>13</v>
+      </c>
+      <c r="T37" s="2">
+        <v>47</v>
+      </c>
     </row>
     <row r="38" spans="1:20" ht="15.75">
       <c r="A38" s="2">
         <v>36</v>
       </c>
       <c r="B38" s="2"/>
-      <c r="T38" s="1"/>
+      <c r="D38" s="2">
+        <v>17</v>
+      </c>
+      <c r="E38" s="2">
+        <v>29</v>
+      </c>
+      <c r="F38" s="2">
+        <v>37</v>
+      </c>
+      <c r="G38" s="2">
+        <v>19</v>
+      </c>
+      <c r="H38" s="2">
+        <v>61</v>
+      </c>
+      <c r="I38" s="2">
+        <v>19</v>
+      </c>
+      <c r="J38" s="2">
+        <v>39</v>
+      </c>
+      <c r="K38" s="2">
+        <v>3</v>
+      </c>
+      <c r="L38" s="2">
+        <v>16</v>
+      </c>
+      <c r="M38" s="2">
+        <v>51</v>
+      </c>
+      <c r="N38" s="2">
+        <v>20</v>
+      </c>
+      <c r="O38" s="2">
+        <v>36</v>
+      </c>
+      <c r="P38" s="2">
+        <v>34</v>
+      </c>
+      <c r="Q38" s="2">
+        <v>62</v>
+      </c>
+      <c r="R38" s="2">
+        <v>63</v>
+      </c>
+      <c r="S38" s="2">
+        <v>53</v>
+      </c>
+      <c r="T38" s="2">
+        <v>31</v>
+      </c>
     </row>
     <row r="39" spans="1:20" ht="15.75">
       <c r="A39" s="2">
         <v>37</v>
       </c>
       <c r="B39" s="2"/>
-      <c r="T39" s="1"/>
+      <c r="D39" s="2">
+        <v>55</v>
+      </c>
+      <c r="E39" s="2">
+        <v>40</v>
+      </c>
+      <c r="F39" s="2">
+        <v>6</v>
+      </c>
+      <c r="G39" s="2">
+        <v>38</v>
+      </c>
+      <c r="H39" s="2">
+        <v>8</v>
+      </c>
+      <c r="I39" s="2">
+        <v>19</v>
+      </c>
+      <c r="J39" s="2">
+        <v>7</v>
+      </c>
+      <c r="K39" s="2">
+        <v>41</v>
+      </c>
+      <c r="L39" s="2">
+        <v>19</v>
+      </c>
+      <c r="M39" s="2">
+        <v>23</v>
+      </c>
+      <c r="N39" s="2">
+        <v>5</v>
+      </c>
+      <c r="O39" s="2">
+        <v>43</v>
+      </c>
+      <c r="P39" s="2">
+        <v>29</v>
+      </c>
+      <c r="Q39" s="2">
+        <v>51</v>
+      </c>
+      <c r="R39" s="2">
+        <v>20</v>
+      </c>
+      <c r="S39" s="2">
+        <v>34</v>
+      </c>
+      <c r="T39" s="2">
+        <v>55</v>
+      </c>
     </row>
     <row r="40" spans="1:20" ht="15.75">
       <c r="A40" s="2">
         <v>19</v>
       </c>
       <c r="B40" s="2"/>
-      <c r="T40" s="1"/>
+      <c r="D40" s="2">
+        <v>38</v>
+      </c>
+      <c r="E40" s="2">
+        <v>19</v>
+      </c>
+      <c r="F40" s="2">
+        <v>3</v>
+      </c>
+      <c r="G40" s="2">
+        <v>54</v>
+      </c>
+      <c r="H40" s="2">
+        <v>50</v>
+      </c>
+      <c r="I40" s="2">
+        <v>48</v>
+      </c>
+      <c r="J40" s="2">
+        <v>2</v>
+      </c>
+      <c r="K40" s="2">
+        <v>11</v>
+      </c>
+      <c r="L40" s="2">
+        <v>25</v>
+      </c>
+      <c r="M40" s="2">
+        <v>27</v>
+      </c>
+      <c r="N40" s="2">
+        <v>20</v>
+      </c>
+      <c r="O40" s="2">
+        <v>5</v>
+      </c>
+      <c r="P40" s="2">
+        <v>61</v>
+      </c>
+      <c r="Q40" s="2">
+        <v>14</v>
+      </c>
+      <c r="R40" s="2">
+        <v>37</v>
+      </c>
+      <c r="S40" s="2">
+        <v>31</v>
+      </c>
+      <c r="T40" s="2">
+        <v>23</v>
+      </c>
     </row>
     <row r="41" spans="1:20" ht="15.75">
       <c r="A41" s="2">
         <v>38</v>
       </c>
       <c r="B41" s="2"/>
-      <c r="T41" s="1"/>
+      <c r="D41" s="2">
+        <v>16</v>
+      </c>
+      <c r="E41" s="2">
+        <v>29</v>
+      </c>
+      <c r="F41" s="2">
+        <v>36</v>
+      </c>
+      <c r="G41" s="2">
+        <v>6</v>
+      </c>
+      <c r="H41" s="2">
+        <v>3</v>
+      </c>
+      <c r="I41" s="2">
+        <v>41</v>
+      </c>
+      <c r="J41" s="2">
+        <v>11</v>
+      </c>
+      <c r="K41" s="2">
+        <v>30</v>
+      </c>
+      <c r="L41" s="2">
+        <v>50</v>
+      </c>
+      <c r="M41" s="2">
+        <v>14</v>
+      </c>
+      <c r="N41" s="2">
+        <v>53</v>
+      </c>
+      <c r="O41" s="2">
+        <v>37</v>
+      </c>
+      <c r="P41" s="2">
+        <v>28</v>
+      </c>
+      <c r="Q41" s="2">
+        <v>19</v>
+      </c>
+      <c r="R41" s="2">
+        <v>52</v>
+      </c>
+      <c r="S41" s="2">
+        <v>20</v>
+      </c>
+      <c r="T41" s="2">
+        <v>51</v>
+      </c>
     </row>
     <row r="42" spans="1:20" ht="15.75">
       <c r="A42" s="2">
         <v>39</v>
       </c>
       <c r="B42" s="2"/>
-      <c r="T42" s="1"/>
+      <c r="D42" s="2">
+        <v>40</v>
+      </c>
+      <c r="E42" s="2">
+        <v>63</v>
+      </c>
+      <c r="F42" s="2">
+        <v>47</v>
+      </c>
+      <c r="G42" s="2">
+        <v>42</v>
+      </c>
+      <c r="H42" s="2">
+        <v>34</v>
+      </c>
+      <c r="I42" s="2">
+        <v>22</v>
+      </c>
+      <c r="J42" s="2">
+        <v>19</v>
+      </c>
+      <c r="K42" s="2">
+        <v>18</v>
+      </c>
+      <c r="L42" s="2">
+        <v>11</v>
+      </c>
+      <c r="M42" s="2">
+        <v>50</v>
+      </c>
+      <c r="N42" s="2">
+        <v>51</v>
+      </c>
+      <c r="O42" s="2">
+        <v>20</v>
+      </c>
+      <c r="P42" s="2">
+        <v>36</v>
+      </c>
+      <c r="Q42" s="2">
+        <v>21</v>
+      </c>
+      <c r="R42" s="2">
+        <v>58</v>
+      </c>
+      <c r="S42" s="2">
+        <v>44</v>
+      </c>
+      <c r="T42" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="43" spans="1:20" ht="15.75">
       <c r="A43" s="2">
         <v>15</v>
       </c>
       <c r="B43" s="2"/>
-      <c r="T43" s="1"/>
+      <c r="D43" s="2">
+        <v>6</v>
+      </c>
+      <c r="E43" s="2">
+        <v>15</v>
+      </c>
+      <c r="F43" s="2">
+        <v>51</v>
+      </c>
+      <c r="G43" s="2">
+        <v>18</v>
+      </c>
+      <c r="H43" s="2">
+        <v>7</v>
+      </c>
+      <c r="I43" s="2">
+        <v>32</v>
+      </c>
+      <c r="J43" s="2">
+        <v>50</v>
+      </c>
+      <c r="K43" s="2">
+        <v>16</v>
+      </c>
+      <c r="L43" s="2">
+        <v>53</v>
+      </c>
+      <c r="M43" s="2">
+        <v>61</v>
+      </c>
+      <c r="N43" s="2">
+        <v>28</v>
+      </c>
+      <c r="O43" s="2">
+        <v>36</v>
+      </c>
+      <c r="P43" s="2">
+        <v>8</v>
+      </c>
+      <c r="Q43" s="2">
+        <v>53</v>
+      </c>
+      <c r="R43" s="2">
+        <v>48</v>
+      </c>
+      <c r="S43" s="2">
+        <v>19</v>
+      </c>
+      <c r="T43" s="2">
+        <v>19</v>
+      </c>
     </row>
     <row r="44" spans="1:20" ht="15.75">
       <c r="A44" s="2">
         <v>26</v>
       </c>
       <c r="B44" s="2"/>
-      <c r="T44" s="1"/>
+      <c r="D44" s="2">
+        <v>34</v>
+      </c>
+      <c r="E44" s="2">
+        <v>20</v>
+      </c>
+      <c r="F44" s="2">
+        <v>59</v>
+      </c>
+      <c r="G44" s="2">
+        <v>12</v>
+      </c>
+      <c r="H44" s="2">
+        <v>30</v>
+      </c>
+      <c r="I44" s="2">
+        <v>35</v>
+      </c>
+      <c r="J44" s="2">
+        <v>53</v>
+      </c>
+      <c r="K44" s="2">
+        <v>47</v>
+      </c>
+      <c r="L44" s="2">
+        <v>56</v>
+      </c>
+      <c r="M44" s="2">
+        <v>2</v>
+      </c>
+      <c r="N44" s="2">
+        <v>4</v>
+      </c>
+      <c r="O44" s="2">
+        <v>8</v>
+      </c>
+      <c r="P44" s="2">
+        <v>38</v>
+      </c>
+      <c r="Q44" s="2">
+        <v>39</v>
+      </c>
+      <c r="R44" s="2">
+        <v>50</v>
+      </c>
+      <c r="S44" s="2">
+        <v>55</v>
+      </c>
+      <c r="T44" s="2">
+        <v>19</v>
+      </c>
     </row>
     <row r="45" spans="1:20" ht="15.75">
       <c r="A45" s="2">
         <v>21</v>
       </c>
       <c r="B45" s="2"/>
-      <c r="T45" s="1"/>
+      <c r="D45" s="2">
+        <v>11</v>
+      </c>
+      <c r="E45" s="2">
+        <v>36</v>
+      </c>
+      <c r="F45" s="2">
+        <v>28</v>
+      </c>
+      <c r="G45" s="2">
+        <v>45</v>
+      </c>
+      <c r="H45" s="2">
+        <v>40</v>
+      </c>
+      <c r="I45" s="2">
+        <v>20</v>
+      </c>
+      <c r="J45" s="2">
+        <v>31</v>
+      </c>
+      <c r="K45" s="2">
+        <v>21</v>
+      </c>
+      <c r="L45" s="2">
+        <v>23</v>
+      </c>
+      <c r="M45" s="2">
+        <v>5</v>
+      </c>
+      <c r="N45" s="2">
+        <v>7</v>
+      </c>
+      <c r="O45" s="2">
+        <v>28</v>
+      </c>
+      <c r="P45" s="2">
+        <v>32</v>
+      </c>
+      <c r="Q45" s="2">
+        <v>37</v>
+      </c>
+      <c r="R45" s="2">
+        <v>57</v>
+      </c>
+      <c r="S45" s="2">
+        <v>15</v>
+      </c>
+      <c r="T45" s="2">
+        <v>16</v>
+      </c>
     </row>
     <row r="46" spans="1:20" ht="15.75">
       <c r="A46" s="2">
         <v>33</v>
       </c>
       <c r="B46" s="2"/>
-      <c r="T46" s="1"/>
+      <c r="D46" s="2">
+        <v>3</v>
+      </c>
+      <c r="E46" s="2">
+        <v>36</v>
+      </c>
+      <c r="F46" s="2">
+        <v>14</v>
+      </c>
+      <c r="G46" s="2">
+        <v>19</v>
+      </c>
+      <c r="H46" s="2">
+        <v>13</v>
+      </c>
+      <c r="I46" s="2">
+        <v>12</v>
+      </c>
+      <c r="J46" s="2">
+        <v>63</v>
+      </c>
+      <c r="K46" s="2">
+        <v>56</v>
+      </c>
+      <c r="L46" s="2">
+        <v>29</v>
+      </c>
+      <c r="M46" s="2">
+        <v>19</v>
+      </c>
+      <c r="N46" s="2">
+        <v>51</v>
+      </c>
+      <c r="O46" s="2">
+        <v>6</v>
+      </c>
+      <c r="P46" s="2">
+        <v>26</v>
+      </c>
+      <c r="Q46" s="2">
+        <v>20</v>
+      </c>
+      <c r="R46" s="2">
+        <v>11</v>
+      </c>
+      <c r="S46" s="2">
+        <v>33</v>
+      </c>
+      <c r="T46" s="2">
+        <v>13</v>
+      </c>
     </row>
     <row r="47" spans="1:20" ht="15.75">
       <c r="A47" s="2">
         <v>13</v>
       </c>
       <c r="B47" s="2"/>
-      <c r="T47" s="1"/>
+      <c r="D47" s="2">
+        <v>19</v>
+      </c>
+      <c r="E47" s="2">
+        <v>19</v>
+      </c>
+      <c r="F47" s="2">
+        <v>33</v>
+      </c>
+      <c r="G47" s="2">
+        <v>26</v>
+      </c>
+      <c r="H47" s="2">
+        <v>56</v>
+      </c>
+      <c r="I47" s="2">
+        <v>40</v>
+      </c>
+      <c r="J47" s="2">
+        <v>26</v>
+      </c>
+      <c r="K47" s="2">
+        <v>36</v>
+      </c>
+      <c r="L47" s="2">
+        <v>9</v>
+      </c>
+      <c r="M47" s="2">
+        <v>23</v>
+      </c>
+      <c r="N47" s="2">
+        <v>41</v>
+      </c>
+      <c r="O47" s="2">
+        <v>1</v>
+      </c>
+      <c r="P47" s="2">
+        <v>14</v>
+      </c>
+      <c r="Q47" s="2">
+        <v>54</v>
+      </c>
+      <c r="R47" s="2">
+        <v>21</v>
+      </c>
+      <c r="S47" s="2">
+        <v>33</v>
+      </c>
+      <c r="T47" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="48" spans="1:20" ht="15.75">
       <c r="A48" s="2">
         <v>22</v>
       </c>
       <c r="B48" s="2"/>
-      <c r="T48" s="1"/>
+      <c r="D48" s="2">
+        <v>11</v>
+      </c>
+      <c r="E48" s="2">
+        <v>51</v>
+      </c>
+      <c r="F48" s="2">
+        <v>10</v>
+      </c>
+      <c r="G48" s="2">
+        <v>17</v>
+      </c>
+      <c r="H48" s="2">
+        <v>26</v>
+      </c>
+      <c r="I48" s="2">
+        <v>29</v>
+      </c>
+      <c r="J48" s="2">
+        <v>43</v>
+      </c>
+      <c r="K48" s="2">
+        <v>48</v>
+      </c>
+      <c r="L48" s="2">
+        <v>20</v>
+      </c>
+      <c r="M48" s="2">
+        <v>46</v>
+      </c>
+      <c r="N48" s="2">
+        <v>27</v>
+      </c>
+      <c r="O48" s="2">
+        <v>23</v>
+      </c>
+      <c r="P48" s="2">
+        <v>20</v>
+      </c>
+      <c r="Q48" s="2">
+        <v>30</v>
+      </c>
+      <c r="R48" s="2">
+        <v>55</v>
+      </c>
+      <c r="S48" s="2">
+        <v>56</v>
+      </c>
+      <c r="T48" s="2">
+        <v>36</v>
+      </c>
     </row>
     <row r="49" spans="1:20" ht="15.75">
       <c r="A49" s="2">
         <v>40</v>
       </c>
       <c r="B49" s="2"/>
-      <c r="T49" s="1"/>
+      <c r="D49" s="2">
+        <v>4</v>
+      </c>
+      <c r="E49" s="2">
+        <v>37</v>
+      </c>
+      <c r="F49" s="2">
+        <v>25</v>
+      </c>
+      <c r="G49" s="2">
+        <v>1</v>
+      </c>
+      <c r="H49" s="2">
+        <v>18</v>
+      </c>
+      <c r="I49" s="2">
+        <v>5</v>
+      </c>
+      <c r="J49" s="2">
+        <v>10</v>
+      </c>
+      <c r="K49" s="2">
+        <v>42</v>
+      </c>
+      <c r="L49" s="2">
+        <v>40</v>
+      </c>
+      <c r="M49" s="2">
+        <v>39</v>
+      </c>
+      <c r="N49" s="2">
+        <v>23</v>
+      </c>
+      <c r="O49" s="2">
+        <v>44</v>
+      </c>
+      <c r="P49" s="2">
+        <v>62</v>
+      </c>
+      <c r="Q49" s="2">
+        <v>11</v>
+      </c>
+      <c r="R49" s="2">
+        <v>31</v>
+      </c>
+      <c r="S49" s="2">
+        <v>58</v>
+      </c>
+      <c r="T49" s="2">
+        <v>19</v>
+      </c>
     </row>
     <row r="50" spans="1:20" ht="15.75">
       <c r="A50" s="2">
         <v>1</v>
       </c>
       <c r="B50" s="2"/>
-      <c r="T50" s="1"/>
     </row>
     <row r="51" spans="1:20" ht="15.75">
       <c r="A51" s="2">
         <v>41</v>
       </c>
       <c r="B51" s="2"/>
-      <c r="T51" s="1"/>
     </row>
     <row r="52" spans="1:20" ht="15.75">
       <c r="A52" s="2">
         <v>42</v>
       </c>
       <c r="B52" s="2"/>
-      <c r="T52" s="1"/>
     </row>
     <row r="53" spans="1:20" ht="15.75">
       <c r="A53" s="2">
         <v>5</v>
       </c>
       <c r="B53" s="2"/>
-      <c r="T53" s="1"/>
     </row>
     <row r="54" spans="1:20" ht="15.75">
       <c r="A54" s="2">
         <v>5</v>
       </c>
       <c r="B54" s="2"/>
-      <c r="T54" s="1"/>
     </row>
     <row r="55" spans="1:20" ht="15.75">
       <c r="A55" s="2">
         <v>43</v>
       </c>
       <c r="B55" s="2"/>
-      <c r="T55" s="1"/>
     </row>
     <row r="56" spans="1:20" ht="15.75">
       <c r="A56" s="2">
         <v>7</v>
       </c>
       <c r="B56" s="2"/>
-      <c r="T56" s="1"/>
     </row>
     <row r="57" spans="1:20" ht="15.75">
       <c r="A57" s="2">
         <v>6</v>
       </c>
       <c r="B57" s="2"/>
-      <c r="T57" s="1"/>
     </row>
     <row r="58" spans="1:20" ht="15.75">
       <c r="A58" s="2">
@@ -4212,8 +5204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BN408"/>
   <sheetViews>
-    <sheetView topLeftCell="A370" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6979,97 +7971,121 @@
       <c r="BM23" s="4"/>
       <c r="BN23" s="4"/>
     </row>
-    <row r="24" spans="1:66" ht="15.75">
+    <row r="24" spans="1:66">
       <c r="A24">
         <v>20</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="4"/>
-      <c r="S24" s="4"/>
-      <c r="T24" s="1"/>
-      <c r="U24" s="4"/>
-      <c r="V24" s="4"/>
-      <c r="W24" s="4"/>
-      <c r="X24" s="4"/>
-      <c r="Y24" s="4"/>
-      <c r="Z24" s="4"/>
-      <c r="AA24" s="4"/>
-      <c r="AB24" s="4"/>
-      <c r="AC24" s="4"/>
-      <c r="AD24" s="4"/>
-      <c r="AE24" s="4"/>
-      <c r="AF24" s="4"/>
-      <c r="AG24" s="4"/>
-      <c r="AH24" s="4"/>
-      <c r="AI24" s="4"/>
-      <c r="AJ24" s="4"/>
-      <c r="AK24" s="4"/>
-      <c r="AL24" s="4"/>
-      <c r="AM24" s="4"/>
-      <c r="AN24" s="4"/>
-      <c r="AO24" s="4"/>
-      <c r="AP24" s="4"/>
-      <c r="AQ24" s="4"/>
-      <c r="AR24" s="4"/>
-      <c r="AS24" s="4"/>
-      <c r="AT24" s="4"/>
-      <c r="AU24" s="4"/>
-      <c r="AV24" s="4"/>
-      <c r="AW24" s="4"/>
-      <c r="AX24" s="4"/>
-      <c r="AY24" s="4"/>
-      <c r="AZ24" s="4"/>
-      <c r="BA24" s="4"/>
-      <c r="BB24" s="4"/>
-      <c r="BC24" s="4"/>
-      <c r="BD24" s="4"/>
-      <c r="BE24" s="4"/>
-      <c r="BF24" s="4"/>
-      <c r="BG24" s="4"/>
-      <c r="BH24" s="4"/>
-      <c r="BI24" s="4"/>
-      <c r="BJ24" s="4"/>
-      <c r="BK24" s="4"/>
-      <c r="BL24" s="4"/>
-      <c r="BM24" s="4"/>
-      <c r="BN24" s="4"/>
-    </row>
-    <row r="25" spans="1:66" ht="15.75">
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="H24">
+        <v>3</v>
+      </c>
+      <c r="I24">
+        <v>4</v>
+      </c>
+      <c r="J24">
+        <v>5</v>
+      </c>
+      <c r="K24">
+        <v>4</v>
+      </c>
+      <c r="L24">
+        <v>6</v>
+      </c>
+      <c r="M24">
+        <v>7</v>
+      </c>
+      <c r="N24">
+        <v>2</v>
+      </c>
+      <c r="O24">
+        <v>8</v>
+      </c>
+      <c r="P24">
+        <v>9</v>
+      </c>
+      <c r="Q24">
+        <v>10</v>
+      </c>
+      <c r="R24">
+        <v>11</v>
+      </c>
+      <c r="S24">
+        <v>12</v>
+      </c>
+      <c r="T24">
+        <v>13</v>
+      </c>
+      <c r="U24">
+        <v>11</v>
+      </c>
+      <c r="V24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:66">
       <c r="A25">
         <v>21</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
-      <c r="P25" s="4"/>
-      <c r="Q25" s="4"/>
-      <c r="R25" s="4"/>
-      <c r="S25" s="4"/>
-      <c r="T25" s="1"/>
-      <c r="U25" s="4"/>
-      <c r="V25" s="4"/>
+      <c r="F25">
+        <v>14</v>
+      </c>
+      <c r="G25">
+        <v>15</v>
+      </c>
+      <c r="H25">
+        <v>16</v>
+      </c>
+      <c r="I25">
+        <v>17</v>
+      </c>
+      <c r="J25">
+        <v>18</v>
+      </c>
+      <c r="K25">
+        <v>19</v>
+      </c>
+      <c r="L25">
+        <v>20</v>
+      </c>
+      <c r="M25">
+        <v>21</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="O25">
+        <v>22</v>
+      </c>
+      <c r="P25">
+        <v>3</v>
+      </c>
+      <c r="Q25">
+        <v>23</v>
+      </c>
+      <c r="R25">
+        <v>24</v>
+      </c>
+      <c r="S25">
+        <v>25</v>
+      </c>
+      <c r="T25">
+        <v>26</v>
+      </c>
+      <c r="U25">
+        <v>19</v>
+      </c>
+      <c r="V25">
+        <v>17</v>
+      </c>
       <c r="W25" s="4"/>
       <c r="X25" s="4"/>
       <c r="Y25" s="4"/>
@@ -7115,29 +8131,63 @@
       <c r="BM25" s="4"/>
       <c r="BN25" s="4"/>
     </row>
-    <row r="26" spans="1:66" ht="15.75">
+    <row r="26" spans="1:66">
       <c r="A26">
         <v>1</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="4"/>
-      <c r="S26" s="4"/>
-      <c r="T26" s="1"/>
-      <c r="U26" s="4"/>
-      <c r="V26" s="4"/>
+      <c r="F26">
+        <v>27</v>
+      </c>
+      <c r="G26">
+        <v>28</v>
+      </c>
+      <c r="H26">
+        <v>19</v>
+      </c>
+      <c r="I26">
+        <v>29</v>
+      </c>
+      <c r="J26">
+        <v>6</v>
+      </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
+      <c r="L26">
+        <v>8</v>
+      </c>
+      <c r="M26">
+        <v>31</v>
+      </c>
+      <c r="N26">
+        <v>26</v>
+      </c>
+      <c r="O26">
+        <v>32</v>
+      </c>
+      <c r="P26">
+        <v>33</v>
+      </c>
+      <c r="Q26">
+        <v>34</v>
+      </c>
+      <c r="R26">
+        <v>35</v>
+      </c>
+      <c r="S26">
+        <v>19</v>
+      </c>
+      <c r="T26">
+        <v>36</v>
+      </c>
+      <c r="U26">
+        <v>37</v>
+      </c>
+      <c r="V26">
+        <v>38</v>
+      </c>
       <c r="W26" s="4"/>
       <c r="X26" s="4"/>
       <c r="Y26" s="4"/>
@@ -7183,29 +8233,63 @@
       <c r="BM26" s="4"/>
       <c r="BN26" s="4"/>
     </row>
-    <row r="27" spans="1:66" ht="15.75">
+    <row r="27" spans="1:66">
       <c r="A27">
         <v>22</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-      <c r="P27" s="4"/>
-      <c r="Q27" s="4"/>
-      <c r="R27" s="4"/>
-      <c r="S27" s="4"/>
-      <c r="T27" s="1"/>
-      <c r="U27" s="4"/>
-      <c r="V27" s="4"/>
+      <c r="F27">
+        <v>39</v>
+      </c>
+      <c r="G27">
+        <v>40</v>
+      </c>
+      <c r="H27">
+        <v>4</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>41</v>
+      </c>
+      <c r="K27">
+        <v>7</v>
+      </c>
+      <c r="L27">
+        <v>3</v>
+      </c>
+      <c r="M27">
+        <v>9</v>
+      </c>
+      <c r="N27">
+        <v>10</v>
+      </c>
+      <c r="O27">
+        <v>42</v>
+      </c>
+      <c r="P27">
+        <v>6</v>
+      </c>
+      <c r="Q27">
+        <v>2</v>
+      </c>
+      <c r="R27">
+        <v>43</v>
+      </c>
+      <c r="S27">
+        <v>10</v>
+      </c>
+      <c r="T27">
+        <v>44</v>
+      </c>
+      <c r="U27">
+        <v>26</v>
+      </c>
+      <c r="V27">
+        <v>45</v>
+      </c>
       <c r="W27" s="4"/>
       <c r="X27" s="4"/>
       <c r="Y27" s="4"/>
@@ -7255,103 +8339,1123 @@
       <c r="A28">
         <v>3</v>
       </c>
+      <c r="F28">
+        <v>8</v>
+      </c>
+      <c r="G28">
+        <v>29</v>
+      </c>
+      <c r="H28">
+        <v>46</v>
+      </c>
+      <c r="I28">
+        <v>27</v>
+      </c>
+      <c r="J28">
+        <v>5</v>
+      </c>
+      <c r="K28">
+        <v>28</v>
+      </c>
+      <c r="L28">
+        <v>47</v>
+      </c>
+      <c r="M28">
+        <v>48</v>
+      </c>
+      <c r="N28">
+        <v>49</v>
+      </c>
+      <c r="O28">
+        <v>12</v>
+      </c>
+      <c r="P28">
+        <v>20</v>
+      </c>
+      <c r="Q28">
+        <v>22</v>
+      </c>
+      <c r="R28">
+        <v>15</v>
+      </c>
+      <c r="S28">
+        <v>14</v>
+      </c>
+      <c r="T28">
+        <v>17</v>
+      </c>
+      <c r="U28">
+        <v>31</v>
+      </c>
+      <c r="V28">
+        <v>19</v>
+      </c>
     </row>
     <row r="29" spans="1:66">
       <c r="A29">
         <v>23</v>
       </c>
+      <c r="F29">
+        <v>23</v>
+      </c>
+      <c r="G29">
+        <v>16</v>
+      </c>
+      <c r="H29">
+        <v>26</v>
+      </c>
+      <c r="I29">
+        <v>18</v>
+      </c>
+      <c r="J29">
+        <v>36</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <v>24</v>
+      </c>
+      <c r="M29">
+        <v>30</v>
+      </c>
+      <c r="N29">
+        <v>38</v>
+      </c>
+      <c r="O29">
+        <v>21</v>
+      </c>
+      <c r="P29">
+        <v>26</v>
+      </c>
+      <c r="Q29">
+        <v>13</v>
+      </c>
+      <c r="R29">
+        <v>31</v>
+      </c>
+      <c r="S29">
+        <v>37</v>
+      </c>
+      <c r="T29">
+        <v>50</v>
+      </c>
+      <c r="U29">
+        <v>39</v>
+      </c>
+      <c r="V29">
+        <v>40</v>
+      </c>
     </row>
     <row r="30" spans="1:66">
       <c r="A30">
         <v>24</v>
       </c>
+      <c r="F30">
+        <v>10</v>
+      </c>
+      <c r="G30">
+        <v>34</v>
+      </c>
+      <c r="H30">
+        <v>33</v>
+      </c>
+      <c r="I30">
+        <v>25</v>
+      </c>
+      <c r="J30">
+        <v>19</v>
+      </c>
+      <c r="K30">
+        <v>45</v>
+      </c>
+      <c r="L30">
+        <v>44</v>
+      </c>
+      <c r="M30">
+        <v>9</v>
+      </c>
+      <c r="N30">
+        <v>31</v>
+      </c>
+      <c r="O30">
+        <v>26</v>
+      </c>
+      <c r="P30">
+        <v>18</v>
+      </c>
+      <c r="Q30">
+        <v>7</v>
+      </c>
+      <c r="R30">
+        <v>32</v>
+      </c>
+      <c r="S30">
+        <v>35</v>
+      </c>
+      <c r="T30">
+        <v>39</v>
+      </c>
+      <c r="U30">
+        <v>41</v>
+      </c>
+      <c r="V30">
+        <v>7</v>
+      </c>
     </row>
     <row r="31" spans="1:66">
       <c r="A31">
         <v>25</v>
       </c>
+      <c r="F31">
+        <v>46</v>
+      </c>
+      <c r="G31">
+        <v>47</v>
+      </c>
+      <c r="H31">
+        <v>4</v>
+      </c>
+      <c r="I31">
+        <v>3</v>
+      </c>
+      <c r="J31">
+        <v>41</v>
+      </c>
+      <c r="K31">
+        <v>7</v>
+      </c>
+      <c r="L31">
+        <v>23</v>
+      </c>
+      <c r="M31">
+        <v>13</v>
+      </c>
+      <c r="N31">
+        <v>26</v>
+      </c>
+      <c r="O31">
+        <v>45</v>
+      </c>
+      <c r="P31">
+        <v>22</v>
+      </c>
+      <c r="Q31">
+        <v>27</v>
+      </c>
+      <c r="R31">
+        <v>6</v>
+      </c>
+      <c r="S31">
+        <v>29</v>
+      </c>
+      <c r="T31">
+        <v>10</v>
+      </c>
+      <c r="U31">
+        <v>10</v>
+      </c>
+      <c r="V31">
+        <v>8</v>
+      </c>
     </row>
     <row r="32" spans="1:66">
       <c r="A32">
         <v>26</v>
       </c>
-    </row>
-    <row r="33" spans="1:1">
+      <c r="F32">
+        <v>51</v>
+      </c>
+      <c r="G32">
+        <v>5</v>
+      </c>
+      <c r="H32">
+        <v>24</v>
+      </c>
+      <c r="I32">
+        <v>26</v>
+      </c>
+      <c r="J32">
+        <v>12</v>
+      </c>
+      <c r="K32">
+        <v>30</v>
+      </c>
+      <c r="L32">
+        <v>38</v>
+      </c>
+      <c r="M32">
+        <v>14</v>
+      </c>
+      <c r="N32">
+        <v>26</v>
+      </c>
+      <c r="O32">
+        <v>25</v>
+      </c>
+      <c r="P32">
+        <v>31</v>
+      </c>
+      <c r="Q32">
+        <v>37</v>
+      </c>
+      <c r="R32">
+        <v>46</v>
+      </c>
+      <c r="S32">
+        <v>27</v>
+      </c>
+      <c r="T32">
+        <v>48</v>
+      </c>
+      <c r="U32">
+        <v>1</v>
+      </c>
+      <c r="V32">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22">
       <c r="A33">
         <v>19</v>
       </c>
-    </row>
-    <row r="34" spans="1:1">
+      <c r="F33">
+        <v>7</v>
+      </c>
+      <c r="G33">
+        <v>3</v>
+      </c>
+      <c r="H33">
+        <v>36</v>
+      </c>
+      <c r="I33">
+        <v>10</v>
+      </c>
+      <c r="J33">
+        <v>16</v>
+      </c>
+      <c r="K33">
+        <v>52</v>
+      </c>
+      <c r="L33">
+        <v>11</v>
+      </c>
+      <c r="M33">
+        <v>21</v>
+      </c>
+      <c r="N33">
+        <v>49</v>
+      </c>
+      <c r="O33">
+        <v>34</v>
+      </c>
+      <c r="P33">
+        <v>40</v>
+      </c>
+      <c r="Q33">
+        <v>17</v>
+      </c>
+      <c r="R33">
+        <v>45</v>
+      </c>
+      <c r="S33">
+        <v>6</v>
+      </c>
+      <c r="T33">
+        <v>22</v>
+      </c>
+      <c r="U33">
+        <v>8</v>
+      </c>
+      <c r="V33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22">
       <c r="A34">
         <v>17</v>
       </c>
-    </row>
-    <row r="35" spans="1:1">
+      <c r="F34">
+        <v>5</v>
+      </c>
+      <c r="G34">
+        <v>51</v>
+      </c>
+      <c r="H34">
+        <v>12</v>
+      </c>
+      <c r="I34">
+        <v>9</v>
+      </c>
+      <c r="J34">
+        <v>15</v>
+      </c>
+      <c r="K34">
+        <v>14</v>
+      </c>
+      <c r="L34">
+        <v>30</v>
+      </c>
+      <c r="M34">
+        <v>37</v>
+      </c>
+      <c r="N34">
+        <v>16</v>
+      </c>
+      <c r="O34">
+        <v>33</v>
+      </c>
+      <c r="P34">
+        <v>46</v>
+      </c>
+      <c r="Q34">
+        <v>38</v>
+      </c>
+      <c r="R34">
+        <v>33</v>
+      </c>
+      <c r="S34">
+        <v>29</v>
+      </c>
+      <c r="T34">
+        <v>10</v>
+      </c>
+      <c r="U34">
+        <v>21</v>
+      </c>
+      <c r="V34">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22">
       <c r="A35">
         <v>27</v>
       </c>
-    </row>
-    <row r="36" spans="1:1">
+      <c r="F35">
+        <v>30</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <v>36</v>
+      </c>
+      <c r="I35">
+        <v>10</v>
+      </c>
+      <c r="J35">
+        <v>53</v>
+      </c>
+      <c r="K35">
+        <v>32</v>
+      </c>
+      <c r="L35">
+        <v>19</v>
+      </c>
+      <c r="M35">
+        <v>48</v>
+      </c>
+      <c r="N35">
+        <v>49</v>
+      </c>
+      <c r="O35">
+        <v>47</v>
+      </c>
+      <c r="P35">
+        <v>17</v>
+      </c>
+      <c r="Q35">
+        <v>4</v>
+      </c>
+      <c r="R35">
+        <v>23</v>
+      </c>
+      <c r="S35">
+        <v>13</v>
+      </c>
+      <c r="T35">
+        <v>28</v>
+      </c>
+      <c r="U35">
+        <v>35</v>
+      </c>
+      <c r="V35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22">
       <c r="A36">
         <v>28</v>
       </c>
-    </row>
-    <row r="37" spans="1:1">
+      <c r="F36">
+        <v>3</v>
+      </c>
+      <c r="G36">
+        <v>37</v>
+      </c>
+      <c r="H36">
+        <v>27</v>
+      </c>
+      <c r="I36">
+        <v>1</v>
+      </c>
+      <c r="J36">
+        <v>10</v>
+      </c>
+      <c r="K36">
+        <v>6</v>
+      </c>
+      <c r="L36">
+        <v>33</v>
+      </c>
+      <c r="M36">
+        <v>2</v>
+      </c>
+      <c r="N36">
+        <v>46</v>
+      </c>
+      <c r="O36">
+        <v>38</v>
+      </c>
+      <c r="P36">
+        <v>34</v>
+      </c>
+      <c r="Q36">
+        <v>15</v>
+      </c>
+      <c r="R36">
+        <v>45</v>
+      </c>
+      <c r="S36">
+        <v>24</v>
+      </c>
+      <c r="T36">
+        <v>22</v>
+      </c>
+      <c r="U36">
+        <v>11</v>
+      </c>
+      <c r="V36">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22">
       <c r="A37">
         <v>19</v>
       </c>
-    </row>
-    <row r="38" spans="1:1">
+      <c r="F37">
+        <v>48</v>
+      </c>
+      <c r="G37">
+        <v>30</v>
+      </c>
+      <c r="H37">
+        <v>25</v>
+      </c>
+      <c r="I37">
+        <v>28</v>
+      </c>
+      <c r="J37">
+        <v>8</v>
+      </c>
+      <c r="K37">
+        <v>37</v>
+      </c>
+      <c r="L37">
+        <v>1</v>
+      </c>
+      <c r="M37">
+        <v>31</v>
+      </c>
+      <c r="N37">
+        <v>46</v>
+      </c>
+      <c r="O37">
+        <v>27</v>
+      </c>
+      <c r="P37">
+        <v>44</v>
+      </c>
+      <c r="Q37">
+        <v>34</v>
+      </c>
+      <c r="R37">
+        <v>42</v>
+      </c>
+      <c r="S37">
+        <v>38</v>
+      </c>
+      <c r="T37">
+        <v>5</v>
+      </c>
+      <c r="U37">
+        <v>40</v>
+      </c>
+      <c r="V37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22">
       <c r="A38">
         <v>29</v>
       </c>
-    </row>
-    <row r="39" spans="1:1">
+      <c r="F38">
+        <v>50</v>
+      </c>
+      <c r="G38">
+        <v>6</v>
+      </c>
+      <c r="H38">
+        <v>12</v>
+      </c>
+      <c r="I38">
+        <v>8</v>
+      </c>
+      <c r="J38">
+        <v>42</v>
+      </c>
+      <c r="K38">
+        <v>1</v>
+      </c>
+      <c r="L38">
+        <v>41</v>
+      </c>
+      <c r="M38">
+        <v>7</v>
+      </c>
+      <c r="N38">
+        <v>15</v>
+      </c>
+      <c r="O38">
+        <v>14</v>
+      </c>
+      <c r="P38">
+        <v>49</v>
+      </c>
+      <c r="Q38">
+        <v>16</v>
+      </c>
+      <c r="R38">
+        <v>15</v>
+      </c>
+      <c r="S38">
+        <v>32</v>
+      </c>
+      <c r="T38">
+        <v>33</v>
+      </c>
+      <c r="U38">
+        <v>9</v>
+      </c>
+      <c r="V38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22">
       <c r="A39">
         <v>6</v>
       </c>
-    </row>
-    <row r="40" spans="1:1">
+      <c r="F39">
+        <v>29</v>
+      </c>
+      <c r="G39">
+        <v>11</v>
+      </c>
+      <c r="H39">
+        <v>39</v>
+      </c>
+      <c r="I39">
+        <v>48</v>
+      </c>
+      <c r="J39">
+        <v>44</v>
+      </c>
+      <c r="K39">
+        <v>43</v>
+      </c>
+      <c r="L39">
+        <v>6</v>
+      </c>
+      <c r="M39">
+        <v>17</v>
+      </c>
+      <c r="N39">
+        <v>21</v>
+      </c>
+      <c r="O39">
+        <v>54</v>
+      </c>
+      <c r="P39">
+        <v>36</v>
+      </c>
+      <c r="Q39">
+        <v>50</v>
+      </c>
+      <c r="R39">
+        <v>18</v>
+      </c>
+      <c r="S39">
+        <v>2</v>
+      </c>
+      <c r="T39">
+        <v>2</v>
+      </c>
+      <c r="U39">
+        <v>30</v>
+      </c>
+      <c r="V39">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22">
       <c r="A40">
         <v>30</v>
       </c>
-    </row>
-    <row r="41" spans="1:1">
+      <c r="F40">
+        <v>34</v>
+      </c>
+      <c r="G40">
+        <v>8</v>
+      </c>
+      <c r="H40">
+        <v>38</v>
+      </c>
+      <c r="I40">
+        <v>39</v>
+      </c>
+      <c r="J40">
+        <v>51</v>
+      </c>
+      <c r="K40">
+        <v>45</v>
+      </c>
+      <c r="L40">
+        <v>4</v>
+      </c>
+      <c r="M40">
+        <v>1</v>
+      </c>
+      <c r="N40">
+        <v>2</v>
+      </c>
+      <c r="O40">
+        <v>2</v>
+      </c>
+      <c r="P40">
+        <v>5</v>
+      </c>
+      <c r="Q40">
+        <v>43</v>
+      </c>
+      <c r="R40">
+        <v>42</v>
+      </c>
+      <c r="S40">
+        <v>3</v>
+      </c>
+      <c r="T40">
+        <v>41</v>
+      </c>
+      <c r="U40">
+        <v>7</v>
+      </c>
+      <c r="V40">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22">
       <c r="A41">
         <v>8</v>
       </c>
-    </row>
-    <row r="42" spans="1:1">
+      <c r="F41">
+        <v>12</v>
+      </c>
+      <c r="G41">
+        <v>17</v>
+      </c>
+      <c r="H41">
+        <v>13</v>
+      </c>
+      <c r="I41">
+        <v>26</v>
+      </c>
+      <c r="J41">
+        <v>14</v>
+      </c>
+      <c r="K41">
+        <v>26</v>
+      </c>
+      <c r="L41">
+        <v>53</v>
+      </c>
+      <c r="M41">
+        <v>20</v>
+      </c>
+      <c r="N41">
+        <v>41</v>
+      </c>
+      <c r="O41">
+        <v>31</v>
+      </c>
+      <c r="P41">
+        <v>51</v>
+      </c>
+      <c r="Q41">
+        <v>16</v>
+      </c>
+      <c r="R41">
+        <v>23</v>
+      </c>
+      <c r="S41">
+        <v>1</v>
+      </c>
+      <c r="T41">
+        <v>42</v>
+      </c>
+      <c r="U41">
+        <v>1</v>
+      </c>
+      <c r="V41">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22">
       <c r="A42">
         <v>31</v>
       </c>
-    </row>
-    <row r="43" spans="1:1">
+      <c r="F42">
+        <v>2</v>
+      </c>
+      <c r="G42">
+        <v>9</v>
+      </c>
+      <c r="H42">
+        <v>32</v>
+      </c>
+      <c r="I42">
+        <v>37</v>
+      </c>
+      <c r="J42">
+        <v>10</v>
+      </c>
+      <c r="K42">
+        <v>6</v>
+      </c>
+      <c r="L42">
+        <v>51</v>
+      </c>
+      <c r="M42">
+        <v>16</v>
+      </c>
+      <c r="N42">
+        <v>53</v>
+      </c>
+      <c r="O42">
+        <v>47</v>
+      </c>
+      <c r="P42">
+        <v>19</v>
+      </c>
+      <c r="Q42">
+        <v>26</v>
+      </c>
+      <c r="R42">
+        <v>53</v>
+      </c>
+      <c r="S42">
+        <v>29</v>
+      </c>
+      <c r="T42">
+        <v>39</v>
+      </c>
+      <c r="U42">
+        <v>26</v>
+      </c>
+      <c r="V42">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22">
       <c r="A43">
         <v>26</v>
       </c>
-    </row>
-    <row r="44" spans="1:1">
+      <c r="F43">
+        <v>15</v>
+      </c>
+      <c r="G43">
+        <v>5</v>
+      </c>
+      <c r="H43">
+        <v>17</v>
+      </c>
+      <c r="I43">
+        <v>18</v>
+      </c>
+      <c r="J43">
+        <v>19</v>
+      </c>
+      <c r="K43">
+        <v>24</v>
+      </c>
+      <c r="L43">
+        <v>45</v>
+      </c>
+      <c r="M43">
+        <v>53</v>
+      </c>
+      <c r="N43">
+        <v>32</v>
+      </c>
+      <c r="O43">
+        <v>19</v>
+      </c>
+      <c r="P43">
+        <v>42</v>
+      </c>
+      <c r="Q43">
+        <v>1</v>
+      </c>
+      <c r="R43">
+        <v>2</v>
+      </c>
+      <c r="S43">
+        <v>41</v>
+      </c>
+      <c r="T43">
+        <v>46</v>
+      </c>
+      <c r="U43">
+        <v>33</v>
+      </c>
+      <c r="V43">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22">
       <c r="A44">
         <v>32</v>
       </c>
-    </row>
-    <row r="45" spans="1:1">
+      <c r="F44">
+        <v>22</v>
+      </c>
+      <c r="G44">
+        <v>25</v>
+      </c>
+      <c r="H44">
+        <v>20</v>
+      </c>
+      <c r="I44">
+        <v>17</v>
+      </c>
+      <c r="J44">
+        <v>13</v>
+      </c>
+      <c r="K44">
+        <v>1</v>
+      </c>
+      <c r="L44">
+        <v>50</v>
+      </c>
+      <c r="M44">
+        <v>13</v>
+      </c>
+      <c r="N44">
+        <v>42</v>
+      </c>
+      <c r="O44">
+        <v>36</v>
+      </c>
+      <c r="P44">
+        <v>47</v>
+      </c>
+      <c r="Q44">
+        <v>19</v>
+      </c>
+      <c r="R44">
+        <v>54</v>
+      </c>
+      <c r="S44">
+        <v>46</v>
+      </c>
+      <c r="T44">
+        <v>25</v>
+      </c>
+      <c r="U44">
+        <v>11</v>
+      </c>
+      <c r="V44">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22">
       <c r="A45">
         <v>33</v>
       </c>
-    </row>
-    <row r="46" spans="1:1">
+      <c r="F45">
+        <v>53</v>
+      </c>
+      <c r="G45">
+        <v>17</v>
+      </c>
+      <c r="H45">
+        <v>47</v>
+      </c>
+      <c r="I45">
+        <v>41</v>
+      </c>
+      <c r="J45">
+        <v>41</v>
+      </c>
+      <c r="K45">
+        <v>21</v>
+      </c>
+      <c r="L45">
+        <v>17</v>
+      </c>
+      <c r="M45">
+        <v>37</v>
+      </c>
+      <c r="N45">
+        <v>3</v>
+      </c>
+      <c r="O45">
+        <v>9</v>
+      </c>
+      <c r="P45">
+        <v>10</v>
+      </c>
+      <c r="Q45">
+        <v>13</v>
+      </c>
+      <c r="R45">
+        <v>35</v>
+      </c>
+      <c r="S45">
+        <v>20</v>
+      </c>
+      <c r="T45">
+        <v>2</v>
+      </c>
+      <c r="U45">
+        <v>18</v>
+      </c>
+      <c r="V45">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22">
       <c r="A46">
         <v>34</v>
       </c>
-    </row>
-    <row r="47" spans="1:1">
+      <c r="F46">
+        <v>5</v>
+      </c>
+      <c r="G46">
+        <v>23</v>
+      </c>
+      <c r="H46">
+        <v>28</v>
+      </c>
+      <c r="I46">
+        <v>32</v>
+      </c>
+      <c r="J46">
+        <v>33</v>
+      </c>
+      <c r="K46">
+        <v>26</v>
+      </c>
+      <c r="L46">
+        <v>53</v>
+      </c>
+      <c r="M46">
+        <v>31</v>
+      </c>
+      <c r="N46">
+        <v>28</v>
+      </c>
+      <c r="O46">
+        <v>30</v>
+      </c>
+      <c r="P46">
+        <v>16</v>
+      </c>
+      <c r="Q46">
+        <v>48</v>
+      </c>
+      <c r="R46">
+        <v>7</v>
+      </c>
+      <c r="S46">
+        <v>3</v>
+      </c>
+      <c r="T46">
+        <v>35</v>
+      </c>
+      <c r="U46">
+        <v>14</v>
+      </c>
+      <c r="V46">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22">
       <c r="A47">
         <v>35</v>
       </c>
-    </row>
-    <row r="48" spans="1:1">
+      <c r="F47">
+        <v>15</v>
+      </c>
+      <c r="G47">
+        <v>45</v>
+      </c>
+      <c r="H47">
+        <v>13</v>
+      </c>
+      <c r="I47">
+        <v>48</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+      <c r="K47">
+        <v>14</v>
+      </c>
+      <c r="L47">
+        <v>30</v>
+      </c>
+      <c r="M47">
+        <v>21</v>
+      </c>
+      <c r="N47">
+        <v>26</v>
+      </c>
+      <c r="O47">
+        <v>45</v>
+      </c>
+      <c r="P47">
+        <v>22</v>
+      </c>
+      <c r="Q47">
+        <v>27</v>
+      </c>
+      <c r="R47">
+        <v>38</v>
+      </c>
+      <c r="S47">
+        <v>11</v>
+      </c>
+      <c r="T47">
+        <v>6</v>
+      </c>
+      <c r="U47">
+        <v>30</v>
+      </c>
+      <c r="V47">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22">
       <c r="A48">
         <v>19</v>
       </c>
@@ -9166,8 +11270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Report development, Results added
Further development of report, added a number of results for tri-gram
fitness, and added some graphs and information to cipher models.
</commit_message>
<xml_diff>
--- a/Documentation/Design/Cipher Models.xlsx
+++ b/Documentation/Design/Cipher Models.xlsx
@@ -4,20 +4,113 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="28755" windowHeight="12585"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="28755" windowHeight="12585" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Z340" sheetId="1" r:id="rId1"/>
     <sheet name="Z408" sheetId="2" r:id="rId2"/>
     <sheet name="Test Substitution" sheetId="3" r:id="rId3"/>
+    <sheet name="English Language Frequency" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+  <si>
+    <t>Character Frequency</t>
+  </si>
+  <si>
+    <t>Character frequency</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>English language letter frequences</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -46,16 +139,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8FAFE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -72,11 +177,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF8F9399"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF8F9399"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF8F9399"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF8F9399"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -90,6 +210,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -97,6 +223,893 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-GB"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Z340</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Character frequency</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Z340'!$C$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Character frequency</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>'Z340'!$D$28:$BN$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="63"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="67988096"/>
+        <c:axId val="68005248"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="67988096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="68005248"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="68005248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="24"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="67988096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="2"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-GB"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Z408 Character Frequency</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Z408'!$C$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Character Frequency</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>'Z408'!$D$21:$BE$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="82427264"/>
+        <c:axId val="82441344"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="82427264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="82441344"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="2"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="82441344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="82427264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-GB"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'English Language Frequency'!$E$6:$E$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>English language letter frequences</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'English Language Frequency'!$D$8:$D$33</c:f>
+              <c:strCache>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>D</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>E</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>F</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>G</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>H</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>I</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>J</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>K</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>L</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>M</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>N</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>O</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>P</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Q</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>R</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>S</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>T</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>U</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>V</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>W</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>X</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Y</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Z</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'English Language Frequency'!$E$8:$E$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>8.1670000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4919999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.7820000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.2529999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.12701999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2280000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0150000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.0940000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.966E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.5299999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.7200000000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.0250000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.4060000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.7489999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.5069999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.9290000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9.5E-4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.987E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.3270000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.0560000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.758E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.7800000000000005E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.3599999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.5E-3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.9740000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7.3999999999999999E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="74192768"/>
+        <c:axId val="74194304"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="74192768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="74194304"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="74194304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="74192768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -384,15 +1397,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BN343"/>
+  <dimension ref="A1:DE343"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K47" sqref="K47"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="2" width="9.140625" style="4"/>
+    <col min="3" max="3" width="19.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:66" ht="15.75">
@@ -2019,7 +3034,7 @@
       <c r="Y16" s="2"/>
       <c r="AC16" s="2"/>
     </row>
-    <row r="17" spans="1:29" ht="15.75">
+    <row r="17" spans="1:66" ht="15.75">
       <c r="A17" s="2">
         <v>17</v>
       </c>
@@ -2040,7 +3055,7 @@
       <c r="AB17" s="2"/>
       <c r="AC17" s="2"/>
     </row>
-    <row r="18" spans="1:29" ht="15.75">
+    <row r="18" spans="1:66" ht="15.75">
       <c r="A18" s="2">
         <v>18</v>
       </c>
@@ -2062,7 +3077,7 @@
       <c r="AB18" s="2"/>
       <c r="AC18" s="2"/>
     </row>
-    <row r="19" spans="1:29" ht="15.75">
+    <row r="19" spans="1:66" ht="15.75">
       <c r="A19" s="2">
         <v>5</v>
       </c>
@@ -2084,7 +3099,7 @@
       <c r="AB19" s="2"/>
       <c r="AC19" s="2"/>
     </row>
-    <row r="20" spans="1:29" ht="15.75">
+    <row r="20" spans="1:66" ht="15.75">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -2106,7 +3121,7 @@
       <c r="AB20" s="2"/>
       <c r="AC20" s="2"/>
     </row>
-    <row r="21" spans="1:29" ht="15.75">
+    <row r="21" spans="1:66" ht="15.75">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -2129,7 +3144,7 @@
       <c r="AB21" s="2"/>
       <c r="AC21" s="2"/>
     </row>
-    <row r="22" spans="1:29" ht="15.75">
+    <row r="22" spans="1:66" ht="15.75">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -2153,7 +3168,7 @@
       <c r="AB22" s="2"/>
       <c r="AC22" s="2"/>
     </row>
-    <row r="23" spans="1:29" ht="15.75">
+    <row r="23" spans="1:66" ht="15.75">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -2177,7 +3192,7 @@
       <c r="AB23" s="2"/>
       <c r="AC23" s="2"/>
     </row>
-    <row r="24" spans="1:29" ht="15.75">
+    <row r="24" spans="1:66" ht="15.75">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -2188,7 +3203,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="25" spans="1:29" ht="15.75">
+    <row r="25" spans="1:66" ht="15.75">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -2199,7 +3214,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="26" spans="1:29" ht="15.75">
+    <row r="26" spans="1:66" ht="15.75">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -2210,7 +3225,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="27" spans="1:29" ht="15.75">
+    <row r="27" spans="1:66" ht="15.75">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -2221,486 +3236,536 @@
         <v>340</v>
       </c>
     </row>
-    <row r="28" spans="1:29" ht="15.75">
+    <row r="28" spans="1:66" ht="15.75">
       <c r="A28" s="2">
         <v>27</v>
       </c>
       <c r="B28" s="2"/>
-      <c r="T28" s="1"/>
-    </row>
-    <row r="29" spans="1:29" ht="15.75">
+      <c r="C28" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" s="4">
+        <f>COUNTA(D4:D27)</f>
+        <v>4</v>
+      </c>
+      <c r="E28" s="4">
+        <f t="shared" ref="E28:BN28" si="0">COUNTA(E4:E27)</f>
+        <v>3</v>
+      </c>
+      <c r="F28" s="4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G28" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H28" s="4">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="I28" s="4">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J28" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="K28" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="L28" s="4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="M28" s="4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="N28" s="4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="O28" s="4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="P28" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="Q28" s="4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="R28" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="S28" s="4">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="T28" s="4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="U28" s="4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="V28" s="4">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="W28" s="4">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="X28" s="4">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="Y28" s="4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="Z28" s="4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="AA28" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AB28" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="AC28" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="AD28" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="AE28" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="AF28" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="AG28" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="AH28" s="4">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="AI28" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="AJ28" s="4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="AK28" s="4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="AL28" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AM28" s="4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="AN28" s="4">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="AO28" s="4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="AP28" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="AQ28" s="4">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="AR28" s="4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="AS28" s="4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="AT28" s="4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="AU28" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="AV28" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AW28" s="4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="AX28" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="AY28" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="AZ28" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="BA28" s="4">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="BB28" s="4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="BC28" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="BD28" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="BE28" s="4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="BF28" s="4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="BG28" s="4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="BH28" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="BI28" s="4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="BJ28" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="BK28" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="BL28" s="4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="BM28" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="BN28" s="4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:66" ht="15.75">
       <c r="A29" s="2">
         <v>28</v>
       </c>
       <c r="B29" s="2"/>
       <c r="T29" s="1"/>
     </row>
-    <row r="30" spans="1:29" ht="15.75">
+    <row r="30" spans="1:66" ht="15.75">
       <c r="A30" s="2">
         <v>29</v>
       </c>
       <c r="B30" s="2"/>
-      <c r="D30" s="2">
-        <v>1</v>
-      </c>
-      <c r="E30" s="2">
-        <v>2</v>
-      </c>
-      <c r="F30" s="2">
-        <v>3</v>
-      </c>
-      <c r="G30" s="2">
-        <v>4</v>
-      </c>
-      <c r="H30" s="2">
-        <v>5</v>
-      </c>
-      <c r="I30" s="2">
-        <v>6</v>
-      </c>
-      <c r="J30" s="2">
-        <v>7</v>
-      </c>
-      <c r="K30" s="2">
-        <v>8</v>
-      </c>
-      <c r="L30" s="2">
-        <v>9</v>
-      </c>
-      <c r="M30" s="2">
-        <v>10</v>
-      </c>
-      <c r="N30" s="2">
-        <v>11</v>
-      </c>
-      <c r="O30" s="2">
-        <v>12</v>
-      </c>
-      <c r="P30" s="2">
-        <v>13</v>
-      </c>
-      <c r="Q30" s="2">
-        <v>14</v>
-      </c>
-      <c r="R30" s="2">
-        <v>15</v>
-      </c>
-      <c r="S30" s="2">
-        <v>16</v>
-      </c>
-      <c r="T30" s="2">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="31" spans="1:29" ht="15.75">
+    </row>
+    <row r="31" spans="1:66" ht="15.75">
       <c r="A31" s="2">
         <v>30</v>
       </c>
       <c r="B31" s="2"/>
-      <c r="D31" s="2">
-        <v>18</v>
-      </c>
-      <c r="E31" s="2">
-        <v>5</v>
-      </c>
-      <c r="F31" s="2">
-        <v>19</v>
-      </c>
-      <c r="G31" s="2">
-        <v>20</v>
-      </c>
-      <c r="H31" s="2">
-        <v>21</v>
-      </c>
-      <c r="I31" s="2">
-        <v>22</v>
-      </c>
-      <c r="J31" s="2">
-        <v>23</v>
-      </c>
-      <c r="K31" s="2">
-        <v>24</v>
-      </c>
-      <c r="L31" s="2">
-        <v>25</v>
-      </c>
-      <c r="M31" s="2">
-        <v>26</v>
-      </c>
-      <c r="N31" s="2">
-        <v>27</v>
-      </c>
-      <c r="O31" s="2">
-        <v>28</v>
-      </c>
-      <c r="P31" s="2">
-        <v>29</v>
-      </c>
-      <c r="Q31" s="2">
-        <v>30</v>
-      </c>
-      <c r="R31" s="2">
-        <v>31</v>
-      </c>
-      <c r="S31" s="2">
-        <v>32</v>
-      </c>
-      <c r="T31" s="2">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" spans="1:29" ht="15.75">
+    </row>
+    <row r="32" spans="1:66" ht="15.75">
       <c r="A32" s="2">
         <v>31</v>
       </c>
       <c r="B32" s="2"/>
-      <c r="D32" s="2">
-        <v>20</v>
-      </c>
-      <c r="E32" s="2">
-        <v>34</v>
-      </c>
-      <c r="F32" s="2">
-        <v>35</v>
-      </c>
-      <c r="G32" s="2">
-        <v>36</v>
-      </c>
-      <c r="H32" s="2">
-        <v>37</v>
-      </c>
-      <c r="I32" s="2">
-        <v>19</v>
-      </c>
-      <c r="J32" s="2">
-        <v>38</v>
-      </c>
-      <c r="K32" s="2">
-        <v>39</v>
-      </c>
-      <c r="L32" s="2">
-        <v>15</v>
-      </c>
-      <c r="M32" s="2">
-        <v>26</v>
-      </c>
-      <c r="N32" s="2">
-        <v>21</v>
-      </c>
-      <c r="O32" s="2">
-        <v>33</v>
-      </c>
-      <c r="P32" s="2">
-        <v>13</v>
-      </c>
-      <c r="Q32" s="2">
-        <v>22</v>
-      </c>
-      <c r="R32" s="2">
-        <v>40</v>
-      </c>
-      <c r="S32" s="2">
-        <v>1</v>
-      </c>
-      <c r="T32" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" ht="15.75">
+    </row>
+    <row r="33" spans="1:109" ht="15.75">
       <c r="A33" s="2">
         <v>32</v>
       </c>
       <c r="B33" s="2"/>
-      <c r="D33" s="2">
-        <v>42</v>
-      </c>
-      <c r="E33" s="2">
-        <v>5</v>
-      </c>
-      <c r="F33" s="2">
-        <v>5</v>
-      </c>
-      <c r="G33" s="2">
-        <v>43</v>
-      </c>
-      <c r="H33" s="2">
-        <v>7</v>
-      </c>
-      <c r="I33" s="2">
-        <v>6</v>
-      </c>
-      <c r="J33" s="2">
-        <v>44</v>
-      </c>
-      <c r="K33" s="2">
-        <v>30</v>
-      </c>
-      <c r="L33" s="2">
-        <v>8</v>
-      </c>
-      <c r="M33" s="2">
-        <v>45</v>
-      </c>
-      <c r="N33" s="2">
-        <v>5</v>
-      </c>
-      <c r="O33" s="2">
-        <v>23</v>
-      </c>
-      <c r="P33" s="2">
-        <v>19</v>
-      </c>
-      <c r="Q33" s="2">
-        <v>19</v>
-      </c>
-      <c r="R33" s="2">
-        <v>3</v>
-      </c>
-      <c r="S33" s="2">
-        <v>31</v>
-      </c>
-      <c r="T33" s="2">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" ht="15.75">
+    </row>
+    <row r="34" spans="1:109" ht="15.75">
       <c r="A34" s="2">
         <v>33</v>
       </c>
       <c r="B34" s="2"/>
       <c r="D34" s="2">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="E34" s="2">
-        <v>47</v>
+        <v>2</v>
       </c>
       <c r="F34" s="2">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="G34" s="2">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="H34" s="2">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="I34" s="2">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="J34" s="2">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="K34" s="2">
+        <v>8</v>
+      </c>
+      <c r="L34" s="2">
+        <v>9</v>
+      </c>
+      <c r="M34" s="2">
+        <v>10</v>
+      </c>
+      <c r="N34" s="2">
+        <v>11</v>
+      </c>
+      <c r="O34" s="2">
+        <v>12</v>
+      </c>
+      <c r="P34" s="2">
+        <v>13</v>
+      </c>
+      <c r="Q34" s="2">
+        <v>14</v>
+      </c>
+      <c r="R34" s="2">
+        <v>15</v>
+      </c>
+      <c r="S34" s="2">
+        <v>16</v>
+      </c>
+      <c r="T34" s="2">
         <v>17</v>
       </c>
-      <c r="L34" s="2">
-        <v>11</v>
-      </c>
-      <c r="M34" s="2">
-        <v>50</v>
-      </c>
-      <c r="N34" s="2">
-        <v>51</v>
-      </c>
-      <c r="O34" s="2">
-        <v>9</v>
-      </c>
-      <c r="P34" s="2">
-        <v>19</v>
-      </c>
-      <c r="Q34" s="2">
-        <v>52</v>
-      </c>
-      <c r="R34" s="2">
-        <v>53</v>
-      </c>
-      <c r="S34" s="2">
-        <v>10</v>
-      </c>
-      <c r="T34" s="2">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" ht="15.75">
+    </row>
+    <row r="35" spans="1:109" ht="15.75">
       <c r="A35" s="2">
         <v>20</v>
       </c>
       <c r="B35" s="2"/>
       <c r="D35" s="2">
+        <v>18</v>
+      </c>
+      <c r="E35" s="2">
         <v>5</v>
       </c>
-      <c r="E35" s="2">
-        <v>44</v>
-      </c>
       <c r="F35" s="2">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="G35" s="2">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="H35" s="2">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="I35" s="2">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="J35" s="2">
         <v>23</v>
       </c>
       <c r="K35" s="2">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="L35" s="2">
+        <v>25</v>
+      </c>
+      <c r="M35" s="2">
+        <v>26</v>
+      </c>
+      <c r="N35" s="2">
+        <v>27</v>
+      </c>
+      <c r="O35" s="2">
+        <v>28</v>
+      </c>
+      <c r="P35" s="2">
+        <v>29</v>
+      </c>
+      <c r="Q35" s="2">
         <v>30</v>
       </c>
-      <c r="M35" s="2">
-        <v>17</v>
-      </c>
-      <c r="N35" s="2">
-        <v>56</v>
-      </c>
-      <c r="O35" s="2">
-        <v>10</v>
-      </c>
-      <c r="P35" s="2">
-        <v>51</v>
-      </c>
-      <c r="Q35" s="2">
-        <v>4</v>
-      </c>
       <c r="R35" s="2">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="S35" s="2">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="T35" s="2">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" ht="15.75">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:109" ht="15.75">
       <c r="A36" s="2">
         <v>34</v>
       </c>
       <c r="B36" s="2"/>
       <c r="D36" s="2">
+        <v>20</v>
+      </c>
+      <c r="E36" s="2">
+        <v>34</v>
+      </c>
+      <c r="F36" s="2">
+        <v>35</v>
+      </c>
+      <c r="G36" s="2">
+        <v>36</v>
+      </c>
+      <c r="H36" s="2">
+        <v>37</v>
+      </c>
+      <c r="I36" s="2">
+        <v>19</v>
+      </c>
+      <c r="J36" s="2">
+        <v>38</v>
+      </c>
+      <c r="K36" s="2">
+        <v>39</v>
+      </c>
+      <c r="L36" s="2">
+        <v>15</v>
+      </c>
+      <c r="M36" s="2">
+        <v>26</v>
+      </c>
+      <c r="N36" s="2">
+        <v>21</v>
+      </c>
+      <c r="O36" s="2">
+        <v>33</v>
+      </c>
+      <c r="P36" s="2">
+        <v>13</v>
+      </c>
+      <c r="Q36" s="2">
         <v>22</v>
-      </c>
-      <c r="E36" s="2">
-        <v>50</v>
-      </c>
-      <c r="F36" s="2">
-        <v>19</v>
-      </c>
-      <c r="G36" s="2">
-        <v>31</v>
-      </c>
-      <c r="H36" s="2">
-        <v>57</v>
-      </c>
-      <c r="I36" s="2">
-        <v>24</v>
-      </c>
-      <c r="J36" s="2">
-        <v>58</v>
-      </c>
-      <c r="K36" s="2">
-        <v>16</v>
-      </c>
-      <c r="L36" s="2">
-        <v>38</v>
-      </c>
-      <c r="M36" s="2">
-        <v>36</v>
-      </c>
-      <c r="N36" s="2">
-        <v>59</v>
-      </c>
-      <c r="O36" s="2">
-        <v>15</v>
-      </c>
-      <c r="P36" s="2">
-        <v>8</v>
-      </c>
-      <c r="Q36" s="2">
-        <v>28</v>
       </c>
       <c r="R36" s="2">
         <v>40</v>
       </c>
       <c r="S36" s="2">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="T36" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" ht="15.75">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:109" ht="15.75">
       <c r="A37" s="2">
         <v>35</v>
       </c>
       <c r="B37" s="2"/>
       <c r="D37" s="2">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="E37" s="2">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F37" s="2">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="G37" s="2">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H37" s="2">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="I37" s="2">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="J37" s="2">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="K37" s="2">
+        <v>30</v>
+      </c>
+      <c r="L37" s="2">
+        <v>8</v>
+      </c>
+      <c r="M37" s="2">
+        <v>45</v>
+      </c>
+      <c r="N37" s="2">
+        <v>5</v>
+      </c>
+      <c r="O37" s="2">
         <v>23</v>
       </c>
-      <c r="L37" s="2">
+      <c r="P37" s="2">
         <v>19</v>
-      </c>
-      <c r="M37" s="2">
-        <v>46</v>
-      </c>
-      <c r="N37" s="2">
-        <v>18</v>
-      </c>
-      <c r="O37" s="2">
-        <v>27</v>
-      </c>
-      <c r="P37" s="2">
-        <v>40</v>
       </c>
       <c r="Q37" s="2">
         <v>19</v>
       </c>
       <c r="R37" s="2">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="S37" s="2">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="T37" s="2">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" ht="15.75">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:109" ht="15.75">
       <c r="A38" s="2">
         <v>36</v>
       </c>
       <c r="B38" s="2"/>
       <c r="D38" s="2">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="E38" s="2">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="F38" s="2">
         <v>37</v>
@@ -2709,613 +3774,676 @@
         <v>19</v>
       </c>
       <c r="H38" s="2">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="I38" s="2">
+        <v>48</v>
+      </c>
+      <c r="J38" s="2">
+        <v>49</v>
+      </c>
+      <c r="K38" s="2">
+        <v>17</v>
+      </c>
+      <c r="L38" s="2">
+        <v>11</v>
+      </c>
+      <c r="M38" s="2">
+        <v>50</v>
+      </c>
+      <c r="N38" s="2">
+        <v>51</v>
+      </c>
+      <c r="O38" s="2">
+        <v>9</v>
+      </c>
+      <c r="P38" s="2">
         <v>19</v>
       </c>
-      <c r="J38" s="2">
-        <v>39</v>
-      </c>
-      <c r="K38" s="2">
-        <v>3</v>
-      </c>
-      <c r="L38" s="2">
-        <v>16</v>
-      </c>
-      <c r="M38" s="2">
-        <v>51</v>
-      </c>
-      <c r="N38" s="2">
-        <v>20</v>
-      </c>
-      <c r="O38" s="2">
-        <v>36</v>
-      </c>
-      <c r="P38" s="2">
-        <v>34</v>
-      </c>
       <c r="Q38" s="2">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="R38" s="2">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="S38" s="2">
-        <v>53</v>
+        <v>10</v>
       </c>
       <c r="T38" s="2">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" ht="15.75">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:109" ht="15.75">
       <c r="A39" s="2">
         <v>37</v>
       </c>
       <c r="B39" s="2"/>
       <c r="D39" s="2">
+        <v>5</v>
+      </c>
+      <c r="E39" s="2">
+        <v>44</v>
+      </c>
+      <c r="F39" s="2">
+        <v>3</v>
+      </c>
+      <c r="G39" s="2">
+        <v>7</v>
+      </c>
+      <c r="H39" s="2">
+        <v>51</v>
+      </c>
+      <c r="I39" s="2">
+        <v>6</v>
+      </c>
+      <c r="J39" s="2">
+        <v>23</v>
+      </c>
+      <c r="K39" s="2">
         <v>55</v>
       </c>
-      <c r="E39" s="2">
-        <v>40</v>
-      </c>
-      <c r="F39" s="2">
-        <v>6</v>
-      </c>
-      <c r="G39" s="2">
-        <v>38</v>
-      </c>
-      <c r="H39" s="2">
-        <v>8</v>
-      </c>
-      <c r="I39" s="2">
-        <v>19</v>
-      </c>
-      <c r="J39" s="2">
-        <v>7</v>
-      </c>
-      <c r="K39" s="2">
-        <v>41</v>
-      </c>
       <c r="L39" s="2">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="M39" s="2">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="N39" s="2">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="O39" s="2">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="P39" s="2">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="Q39" s="2">
-        <v>51</v>
+        <v>4</v>
       </c>
       <c r="R39" s="2">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="S39" s="2">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="T39" s="2">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" ht="15.75">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:109" ht="15.75">
       <c r="A40" s="2">
         <v>19</v>
       </c>
       <c r="B40" s="2"/>
       <c r="D40" s="2">
+        <v>22</v>
+      </c>
+      <c r="E40" s="2">
+        <v>50</v>
+      </c>
+      <c r="F40" s="2">
+        <v>19</v>
+      </c>
+      <c r="G40" s="2">
+        <v>31</v>
+      </c>
+      <c r="H40" s="2">
+        <v>57</v>
+      </c>
+      <c r="I40" s="2">
+        <v>24</v>
+      </c>
+      <c r="J40" s="2">
+        <v>58</v>
+      </c>
+      <c r="K40" s="2">
+        <v>16</v>
+      </c>
+      <c r="L40" s="2">
         <v>38</v>
       </c>
-      <c r="E40" s="2">
-        <v>19</v>
-      </c>
-      <c r="F40" s="2">
-        <v>3</v>
-      </c>
-      <c r="G40" s="2">
-        <v>54</v>
-      </c>
-      <c r="H40" s="2">
-        <v>50</v>
-      </c>
-      <c r="I40" s="2">
-        <v>48</v>
-      </c>
-      <c r="J40" s="2">
-        <v>2</v>
-      </c>
-      <c r="K40" s="2">
+      <c r="M40" s="2">
+        <v>36</v>
+      </c>
+      <c r="N40" s="2">
+        <v>59</v>
+      </c>
+      <c r="O40" s="2">
+        <v>15</v>
+      </c>
+      <c r="P40" s="2">
+        <v>8</v>
+      </c>
+      <c r="Q40" s="2">
+        <v>28</v>
+      </c>
+      <c r="R40" s="2">
+        <v>40</v>
+      </c>
+      <c r="S40" s="2">
+        <v>13</v>
+      </c>
+      <c r="T40" s="2">
         <v>11</v>
       </c>
-      <c r="L40" s="2">
-        <v>25</v>
-      </c>
-      <c r="M40" s="2">
-        <v>27</v>
-      </c>
-      <c r="N40" s="2">
-        <v>20</v>
-      </c>
-      <c r="O40" s="2">
-        <v>5</v>
-      </c>
-      <c r="P40" s="2">
-        <v>61</v>
-      </c>
-      <c r="Q40" s="2">
-        <v>14</v>
-      </c>
-      <c r="R40" s="2">
-        <v>37</v>
-      </c>
-      <c r="S40" s="2">
-        <v>31</v>
-      </c>
-      <c r="T40" s="2">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" ht="15.75">
+    </row>
+    <row r="41" spans="1:109" ht="15.75">
       <c r="A41" s="2">
         <v>38</v>
       </c>
       <c r="B41" s="2"/>
       <c r="D41" s="2">
+        <v>21</v>
+      </c>
+      <c r="E41" s="2">
+        <v>15</v>
+      </c>
+      <c r="F41" s="2">
         <v>16</v>
       </c>
-      <c r="E41" s="2">
-        <v>29</v>
-      </c>
-      <c r="F41" s="2">
-        <v>36</v>
-      </c>
       <c r="G41" s="2">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="H41" s="2">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="I41" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="J41" s="2">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="K41" s="2">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="L41" s="2">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="M41" s="2">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="N41" s="2">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="O41" s="2">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="P41" s="2">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="Q41" s="2">
         <v>19</v>
       </c>
       <c r="R41" s="2">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="S41" s="2">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="T41" s="2">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20" ht="15.75">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:109" ht="15.75">
       <c r="A42" s="2">
         <v>39</v>
       </c>
       <c r="B42" s="2"/>
       <c r="D42" s="2">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="E42" s="2">
+        <v>29</v>
+      </c>
+      <c r="F42" s="2">
+        <v>37</v>
+      </c>
+      <c r="G42" s="2">
+        <v>19</v>
+      </c>
+      <c r="H42" s="2">
+        <v>61</v>
+      </c>
+      <c r="I42" s="2">
+        <v>19</v>
+      </c>
+      <c r="J42" s="2">
+        <v>39</v>
+      </c>
+      <c r="K42" s="2">
+        <v>3</v>
+      </c>
+      <c r="L42" s="2">
+        <v>16</v>
+      </c>
+      <c r="M42" s="2">
+        <v>51</v>
+      </c>
+      <c r="N42" s="2">
+        <v>20</v>
+      </c>
+      <c r="O42" s="2">
+        <v>36</v>
+      </c>
+      <c r="P42" s="2">
+        <v>34</v>
+      </c>
+      <c r="Q42" s="2">
+        <v>62</v>
+      </c>
+      <c r="R42" s="2">
         <v>63</v>
       </c>
-      <c r="F42" s="2">
-        <v>47</v>
-      </c>
-      <c r="G42" s="2">
-        <v>42</v>
-      </c>
-      <c r="H42" s="2">
-        <v>34</v>
-      </c>
-      <c r="I42" s="2">
-        <v>22</v>
-      </c>
-      <c r="J42" s="2">
-        <v>19</v>
-      </c>
-      <c r="K42" s="2">
-        <v>18</v>
-      </c>
-      <c r="L42" s="2">
-        <v>11</v>
-      </c>
-      <c r="M42" s="2">
-        <v>50</v>
-      </c>
-      <c r="N42" s="2">
-        <v>51</v>
-      </c>
-      <c r="O42" s="2">
-        <v>20</v>
-      </c>
-      <c r="P42" s="2">
-        <v>36</v>
-      </c>
-      <c r="Q42" s="2">
-        <v>21</v>
-      </c>
-      <c r="R42" s="2">
-        <v>58</v>
-      </c>
       <c r="S42" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="T42" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" ht="15.75">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="43" spans="1:109" ht="15.75">
       <c r="A43" s="2">
         <v>15</v>
       </c>
       <c r="B43" s="2"/>
       <c r="D43" s="2">
+        <v>55</v>
+      </c>
+      <c r="E43" s="2">
+        <v>40</v>
+      </c>
+      <c r="F43" s="2">
         <v>6</v>
       </c>
-      <c r="E43" s="2">
-        <v>15</v>
-      </c>
-      <c r="F43" s="2">
+      <c r="G43" s="2">
+        <v>38</v>
+      </c>
+      <c r="H43" s="2">
+        <v>8</v>
+      </c>
+      <c r="I43" s="2">
+        <v>19</v>
+      </c>
+      <c r="J43" s="2">
+        <v>7</v>
+      </c>
+      <c r="K43" s="2">
+        <v>41</v>
+      </c>
+      <c r="L43" s="2">
+        <v>19</v>
+      </c>
+      <c r="M43" s="2">
+        <v>23</v>
+      </c>
+      <c r="N43" s="2">
+        <v>5</v>
+      </c>
+      <c r="O43" s="2">
+        <v>43</v>
+      </c>
+      <c r="P43" s="2">
+        <v>29</v>
+      </c>
+      <c r="Q43" s="2">
         <v>51</v>
       </c>
-      <c r="G43" s="2">
-        <v>18</v>
-      </c>
-      <c r="H43" s="2">
-        <v>7</v>
-      </c>
-      <c r="I43" s="2">
-        <v>32</v>
-      </c>
-      <c r="J43" s="2">
-        <v>50</v>
-      </c>
-      <c r="K43" s="2">
-        <v>16</v>
-      </c>
-      <c r="L43" s="2">
-        <v>53</v>
-      </c>
-      <c r="M43" s="2">
-        <v>61</v>
-      </c>
-      <c r="N43" s="2">
-        <v>28</v>
-      </c>
-      <c r="O43" s="2">
-        <v>36</v>
-      </c>
-      <c r="P43" s="2">
-        <v>8</v>
-      </c>
-      <c r="Q43" s="2">
-        <v>53</v>
-      </c>
       <c r="R43" s="2">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="S43" s="2">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="T43" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" ht="15.75">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:109" ht="15.75">
       <c r="A44" s="2">
         <v>26</v>
       </c>
       <c r="B44" s="2"/>
       <c r="D44" s="2">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E44" s="2">
+        <v>19</v>
+      </c>
+      <c r="F44" s="2">
+        <v>3</v>
+      </c>
+      <c r="G44" s="2">
+        <v>54</v>
+      </c>
+      <c r="H44" s="2">
+        <v>50</v>
+      </c>
+      <c r="I44" s="2">
+        <v>48</v>
+      </c>
+      <c r="J44" s="2">
+        <v>2</v>
+      </c>
+      <c r="K44" s="2">
+        <v>11</v>
+      </c>
+      <c r="L44" s="2">
+        <v>25</v>
+      </c>
+      <c r="M44" s="2">
+        <v>27</v>
+      </c>
+      <c r="N44" s="2">
         <v>20</v>
       </c>
-      <c r="F44" s="2">
-        <v>59</v>
-      </c>
-      <c r="G44" s="2">
-        <v>12</v>
-      </c>
-      <c r="H44" s="2">
-        <v>30</v>
-      </c>
-      <c r="I44" s="2">
-        <v>35</v>
-      </c>
-      <c r="J44" s="2">
-        <v>53</v>
-      </c>
-      <c r="K44" s="2">
-        <v>47</v>
-      </c>
-      <c r="L44" s="2">
-        <v>56</v>
-      </c>
-      <c r="M44" s="2">
-        <v>2</v>
-      </c>
-      <c r="N44" s="2">
-        <v>4</v>
-      </c>
       <c r="O44" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="P44" s="2">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="Q44" s="2">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="R44" s="2">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="S44" s="2">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="T44" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="45" spans="1:20" ht="15.75">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:109" ht="15.75">
       <c r="A45" s="2">
         <v>21</v>
       </c>
       <c r="B45" s="2"/>
       <c r="D45" s="2">
+        <v>16</v>
+      </c>
+      <c r="E45" s="2">
+        <v>29</v>
+      </c>
+      <c r="F45" s="2">
+        <v>36</v>
+      </c>
+      <c r="G45" s="2">
+        <v>6</v>
+      </c>
+      <c r="H45" s="2">
+        <v>3</v>
+      </c>
+      <c r="I45" s="2">
+        <v>41</v>
+      </c>
+      <c r="J45" s="2">
         <v>11</v>
       </c>
-      <c r="E45" s="2">
-        <v>36</v>
-      </c>
-      <c r="F45" s="2">
+      <c r="K45" s="2">
+        <v>30</v>
+      </c>
+      <c r="L45" s="2">
+        <v>50</v>
+      </c>
+      <c r="M45" s="2">
+        <v>14</v>
+      </c>
+      <c r="N45" s="2">
+        <v>53</v>
+      </c>
+      <c r="O45" s="2">
+        <v>37</v>
+      </c>
+      <c r="P45" s="2">
         <v>28</v>
       </c>
-      <c r="G45" s="2">
-        <v>45</v>
-      </c>
-      <c r="H45" s="2">
-        <v>40</v>
-      </c>
-      <c r="I45" s="2">
+      <c r="Q45" s="2">
+        <v>19</v>
+      </c>
+      <c r="R45" s="2">
+        <v>52</v>
+      </c>
+      <c r="S45" s="2">
         <v>20</v>
       </c>
-      <c r="J45" s="2">
-        <v>31</v>
-      </c>
-      <c r="K45" s="2">
-        <v>21</v>
-      </c>
-      <c r="L45" s="2">
-        <v>23</v>
-      </c>
-      <c r="M45" s="2">
-        <v>5</v>
-      </c>
-      <c r="N45" s="2">
-        <v>7</v>
-      </c>
-      <c r="O45" s="2">
-        <v>28</v>
-      </c>
-      <c r="P45" s="2">
-        <v>32</v>
-      </c>
-      <c r="Q45" s="2">
-        <v>37</v>
-      </c>
-      <c r="R45" s="2">
-        <v>57</v>
-      </c>
-      <c r="S45" s="2">
-        <v>15</v>
-      </c>
       <c r="T45" s="2">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="46" spans="1:20" ht="15.75">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="1:109" ht="15.75">
       <c r="A46" s="2">
         <v>33</v>
       </c>
       <c r="B46" s="2"/>
       <c r="D46" s="2">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="E46" s="2">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="F46" s="2">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="G46" s="2">
+        <v>42</v>
+      </c>
+      <c r="H46" s="2">
+        <v>34</v>
+      </c>
+      <c r="I46" s="2">
+        <v>22</v>
+      </c>
+      <c r="J46" s="2">
         <v>19</v>
       </c>
-      <c r="H46" s="2">
-        <v>13</v>
-      </c>
-      <c r="I46" s="2">
-        <v>12</v>
-      </c>
-      <c r="J46" s="2">
-        <v>63</v>
-      </c>
       <c r="K46" s="2">
-        <v>56</v>
+        <v>18</v>
       </c>
       <c r="L46" s="2">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="M46" s="2">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="N46" s="2">
         <v>51</v>
       </c>
       <c r="O46" s="2">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="P46" s="2">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="Q46" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="R46" s="2">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="S46" s="2">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="T46" s="2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="47" spans="1:20" ht="15.75">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:109" ht="15.75">
       <c r="A47" s="2">
         <v>13</v>
       </c>
       <c r="B47" s="2"/>
       <c r="D47" s="2">
+        <v>6</v>
+      </c>
+      <c r="E47" s="2">
+        <v>15</v>
+      </c>
+      <c r="F47" s="2">
+        <v>51</v>
+      </c>
+      <c r="G47" s="2">
+        <v>18</v>
+      </c>
+      <c r="H47" s="2">
+        <v>7</v>
+      </c>
+      <c r="I47" s="2">
+        <v>32</v>
+      </c>
+      <c r="J47" s="2">
+        <v>50</v>
+      </c>
+      <c r="K47" s="2">
+        <v>16</v>
+      </c>
+      <c r="L47" s="2">
+        <v>53</v>
+      </c>
+      <c r="M47" s="2">
+        <v>61</v>
+      </c>
+      <c r="N47" s="2">
+        <v>28</v>
+      </c>
+      <c r="O47" s="2">
+        <v>36</v>
+      </c>
+      <c r="P47" s="2">
+        <v>8</v>
+      </c>
+      <c r="Q47" s="2">
+        <v>53</v>
+      </c>
+      <c r="R47" s="2">
+        <v>48</v>
+      </c>
+      <c r="S47" s="2">
         <v>19</v>
       </c>
-      <c r="E47" s="2">
+      <c r="T47" s="2">
         <v>19</v>
       </c>
-      <c r="F47" s="2">
-        <v>33</v>
-      </c>
-      <c r="G47" s="2">
-        <v>26</v>
-      </c>
-      <c r="H47" s="2">
-        <v>56</v>
-      </c>
-      <c r="I47" s="2">
-        <v>40</v>
-      </c>
-      <c r="J47" s="2">
-        <v>26</v>
-      </c>
-      <c r="K47" s="2">
-        <v>36</v>
-      </c>
-      <c r="L47" s="2">
-        <v>9</v>
-      </c>
-      <c r="M47" s="2">
-        <v>23</v>
-      </c>
-      <c r="N47" s="2">
-        <v>41</v>
-      </c>
-      <c r="O47" s="2">
-        <v>1</v>
-      </c>
-      <c r="P47" s="2">
-        <v>14</v>
-      </c>
-      <c r="Q47" s="2">
-        <v>54</v>
-      </c>
-      <c r="R47" s="2">
-        <v>21</v>
-      </c>
-      <c r="S47" s="2">
-        <v>33</v>
-      </c>
-      <c r="T47" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:20" ht="15.75">
+      <c r="AU47" s="5"/>
+      <c r="AV47" s="5"/>
+      <c r="AW47" s="5"/>
+      <c r="AX47" s="5"/>
+      <c r="AY47" s="5"/>
+      <c r="AZ47" s="5"/>
+      <c r="BA47" s="5"/>
+      <c r="BB47" s="5"/>
+      <c r="BC47" s="5"/>
+      <c r="BD47" s="5"/>
+      <c r="BE47" s="5"/>
+      <c r="BF47" s="5"/>
+      <c r="BG47" s="5"/>
+      <c r="BH47" s="5"/>
+      <c r="BI47" s="5"/>
+      <c r="BJ47" s="5"/>
+      <c r="BK47" s="5"/>
+      <c r="BL47" s="5"/>
+      <c r="BM47" s="5"/>
+      <c r="BN47" s="5"/>
+      <c r="BO47" s="5"/>
+      <c r="BP47" s="5"/>
+      <c r="BQ47" s="5"/>
+      <c r="BR47" s="5"/>
+      <c r="BS47" s="5"/>
+      <c r="BT47" s="5"/>
+      <c r="BU47" s="5"/>
+      <c r="BV47" s="5"/>
+      <c r="BW47" s="5"/>
+      <c r="BX47" s="5"/>
+      <c r="BY47" s="5"/>
+      <c r="BZ47" s="5"/>
+      <c r="CA47" s="5"/>
+      <c r="CB47" s="5"/>
+      <c r="CC47" s="5"/>
+      <c r="CD47" s="5"/>
+      <c r="CE47" s="5"/>
+      <c r="CF47" s="5"/>
+      <c r="CG47" s="5"/>
+      <c r="CH47" s="5"/>
+      <c r="CI47" s="5"/>
+      <c r="CJ47" s="5"/>
+      <c r="CK47" s="5"/>
+      <c r="CL47" s="5"/>
+      <c r="CM47" s="5"/>
+      <c r="CN47" s="5"/>
+      <c r="CO47" s="5"/>
+      <c r="CP47" s="5"/>
+      <c r="CQ47" s="5"/>
+      <c r="CR47" s="5"/>
+      <c r="CS47" s="5"/>
+      <c r="CT47" s="5"/>
+      <c r="CU47" s="5"/>
+      <c r="CV47" s="5"/>
+      <c r="CW47" s="5"/>
+      <c r="CX47" s="5"/>
+      <c r="CY47" s="5"/>
+      <c r="CZ47" s="5"/>
+      <c r="DA47" s="5"/>
+      <c r="DB47" s="5"/>
+      <c r="DC47" s="5"/>
+      <c r="DD47" s="5"/>
+      <c r="DE47" s="5"/>
+    </row>
+    <row r="48" spans="1:109" ht="15.75">
       <c r="A48" s="2">
         <v>22</v>
       </c>
       <c r="B48" s="2"/>
       <c r="D48" s="2">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="E48" s="2">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="F48" s="2">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="G48" s="2">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H48" s="2">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="I48" s="2">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J48" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="K48" s="2">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L48" s="2">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="M48" s="2">
-        <v>46</v>
+        <v>2</v>
       </c>
       <c r="N48" s="2">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="O48" s="2">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="P48" s="2">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="Q48" s="2">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="R48" s="2">
+        <v>50</v>
+      </c>
+      <c r="S48" s="2">
         <v>55</v>
       </c>
-      <c r="S48" s="2">
-        <v>56</v>
-      </c>
       <c r="T48" s="2">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="49" spans="1:20" ht="15.75">
@@ -3324,55 +4452,55 @@
       </c>
       <c r="B49" s="2"/>
       <c r="D49" s="2">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E49" s="2">
+        <v>36</v>
+      </c>
+      <c r="F49" s="2">
+        <v>28</v>
+      </c>
+      <c r="G49" s="2">
+        <v>45</v>
+      </c>
+      <c r="H49" s="2">
+        <v>40</v>
+      </c>
+      <c r="I49" s="2">
+        <v>20</v>
+      </c>
+      <c r="J49" s="2">
+        <v>31</v>
+      </c>
+      <c r="K49" s="2">
+        <v>21</v>
+      </c>
+      <c r="L49" s="2">
+        <v>23</v>
+      </c>
+      <c r="M49" s="2">
+        <v>5</v>
+      </c>
+      <c r="N49" s="2">
+        <v>7</v>
+      </c>
+      <c r="O49" s="2">
+        <v>28</v>
+      </c>
+      <c r="P49" s="2">
+        <v>32</v>
+      </c>
+      <c r="Q49" s="2">
         <v>37</v>
       </c>
-      <c r="F49" s="2">
-        <v>25</v>
-      </c>
-      <c r="G49" s="2">
-        <v>1</v>
-      </c>
-      <c r="H49" s="2">
-        <v>18</v>
-      </c>
-      <c r="I49" s="2">
-        <v>5</v>
-      </c>
-      <c r="J49" s="2">
-        <v>10</v>
-      </c>
-      <c r="K49" s="2">
-        <v>42</v>
-      </c>
-      <c r="L49" s="2">
-        <v>40</v>
-      </c>
-      <c r="M49" s="2">
-        <v>39</v>
-      </c>
-      <c r="N49" s="2">
-        <v>23</v>
-      </c>
-      <c r="O49" s="2">
-        <v>44</v>
-      </c>
-      <c r="P49" s="2">
-        <v>62</v>
-      </c>
-      <c r="Q49" s="2">
-        <v>11</v>
-      </c>
       <c r="R49" s="2">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="S49" s="2">
-        <v>58</v>
+        <v>15</v>
       </c>
       <c r="T49" s="2">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="50" spans="1:20" ht="15.75">
@@ -3380,24 +4508,228 @@
         <v>1</v>
       </c>
       <c r="B50" s="2"/>
+      <c r="D50" s="2">
+        <v>3</v>
+      </c>
+      <c r="E50" s="2">
+        <v>36</v>
+      </c>
+      <c r="F50" s="2">
+        <v>14</v>
+      </c>
+      <c r="G50" s="2">
+        <v>19</v>
+      </c>
+      <c r="H50" s="2">
+        <v>13</v>
+      </c>
+      <c r="I50" s="2">
+        <v>12</v>
+      </c>
+      <c r="J50" s="2">
+        <v>63</v>
+      </c>
+      <c r="K50" s="2">
+        <v>56</v>
+      </c>
+      <c r="L50" s="2">
+        <v>29</v>
+      </c>
+      <c r="M50" s="2">
+        <v>19</v>
+      </c>
+      <c r="N50" s="2">
+        <v>51</v>
+      </c>
+      <c r="O50" s="2">
+        <v>6</v>
+      </c>
+      <c r="P50" s="2">
+        <v>26</v>
+      </c>
+      <c r="Q50" s="2">
+        <v>20</v>
+      </c>
+      <c r="R50" s="2">
+        <v>11</v>
+      </c>
+      <c r="S50" s="2">
+        <v>33</v>
+      </c>
+      <c r="T50" s="2">
+        <v>13</v>
+      </c>
     </row>
     <row r="51" spans="1:20" ht="15.75">
       <c r="A51" s="2">
         <v>41</v>
       </c>
       <c r="B51" s="2"/>
+      <c r="D51" s="2">
+        <v>19</v>
+      </c>
+      <c r="E51" s="2">
+        <v>19</v>
+      </c>
+      <c r="F51" s="2">
+        <v>33</v>
+      </c>
+      <c r="G51" s="2">
+        <v>26</v>
+      </c>
+      <c r="H51" s="2">
+        <v>56</v>
+      </c>
+      <c r="I51" s="2">
+        <v>40</v>
+      </c>
+      <c r="J51" s="2">
+        <v>26</v>
+      </c>
+      <c r="K51" s="2">
+        <v>36</v>
+      </c>
+      <c r="L51" s="2">
+        <v>9</v>
+      </c>
+      <c r="M51" s="2">
+        <v>23</v>
+      </c>
+      <c r="N51" s="2">
+        <v>41</v>
+      </c>
+      <c r="O51" s="2">
+        <v>1</v>
+      </c>
+      <c r="P51" s="2">
+        <v>14</v>
+      </c>
+      <c r="Q51" s="2">
+        <v>54</v>
+      </c>
+      <c r="R51" s="2">
+        <v>21</v>
+      </c>
+      <c r="S51" s="2">
+        <v>33</v>
+      </c>
+      <c r="T51" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="52" spans="1:20" ht="15.75">
       <c r="A52" s="2">
         <v>42</v>
       </c>
       <c r="B52" s="2"/>
+      <c r="D52" s="2">
+        <v>11</v>
+      </c>
+      <c r="E52" s="2">
+        <v>51</v>
+      </c>
+      <c r="F52" s="2">
+        <v>10</v>
+      </c>
+      <c r="G52" s="2">
+        <v>17</v>
+      </c>
+      <c r="H52" s="2">
+        <v>26</v>
+      </c>
+      <c r="I52" s="2">
+        <v>29</v>
+      </c>
+      <c r="J52" s="2">
+        <v>43</v>
+      </c>
+      <c r="K52" s="2">
+        <v>48</v>
+      </c>
+      <c r="L52" s="2">
+        <v>20</v>
+      </c>
+      <c r="M52" s="2">
+        <v>46</v>
+      </c>
+      <c r="N52" s="2">
+        <v>27</v>
+      </c>
+      <c r="O52" s="2">
+        <v>23</v>
+      </c>
+      <c r="P52" s="2">
+        <v>20</v>
+      </c>
+      <c r="Q52" s="2">
+        <v>30</v>
+      </c>
+      <c r="R52" s="2">
+        <v>55</v>
+      </c>
+      <c r="S52" s="2">
+        <v>56</v>
+      </c>
+      <c r="T52" s="2">
+        <v>36</v>
+      </c>
     </row>
     <row r="53" spans="1:20" ht="15.75">
       <c r="A53" s="2">
         <v>5</v>
       </c>
       <c r="B53" s="2"/>
+      <c r="D53" s="2">
+        <v>4</v>
+      </c>
+      <c r="E53" s="2">
+        <v>37</v>
+      </c>
+      <c r="F53" s="2">
+        <v>25</v>
+      </c>
+      <c r="G53" s="2">
+        <v>1</v>
+      </c>
+      <c r="H53" s="2">
+        <v>18</v>
+      </c>
+      <c r="I53" s="2">
+        <v>5</v>
+      </c>
+      <c r="J53" s="2">
+        <v>10</v>
+      </c>
+      <c r="K53" s="2">
+        <v>42</v>
+      </c>
+      <c r="L53" s="2">
+        <v>40</v>
+      </c>
+      <c r="M53" s="2">
+        <v>39</v>
+      </c>
+      <c r="N53" s="2">
+        <v>23</v>
+      </c>
+      <c r="O53" s="2">
+        <v>44</v>
+      </c>
+      <c r="P53" s="2">
+        <v>62</v>
+      </c>
+      <c r="Q53" s="2">
+        <v>11</v>
+      </c>
+      <c r="R53" s="2">
+        <v>31</v>
+      </c>
+      <c r="S53" s="2">
+        <v>58</v>
+      </c>
+      <c r="T53" s="2">
+        <v>19</v>
+      </c>
     </row>
     <row r="54" spans="1:20" ht="15.75">
       <c r="A54" s="2">
@@ -5197,6 +6529,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5204,11 +6537,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BN408"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AD43" sqref="AD43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:66">
       <c r="A1">
@@ -7767,64 +9103,229 @@
       <c r="BM20" s="4"/>
       <c r="BN20" s="4"/>
     </row>
-    <row r="21" spans="1:66" ht="15.75">
+    <row r="21" spans="1:66">
       <c r="A21">
         <v>17</v>
       </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="2"/>
-      <c r="R21" s="2"/>
-      <c r="S21" s="2"/>
-      <c r="T21" s="2"/>
-      <c r="U21" s="2"/>
-      <c r="V21" s="4"/>
-      <c r="W21" s="2"/>
-      <c r="X21" s="2"/>
-      <c r="Y21" s="2"/>
-      <c r="Z21" s="2"/>
-      <c r="AA21" s="4"/>
-      <c r="AB21" s="2"/>
-      <c r="AC21" s="4"/>
-      <c r="AD21" s="4"/>
-      <c r="AE21" s="4"/>
-      <c r="AF21" s="4"/>
-      <c r="AG21" s="4"/>
-      <c r="AH21" s="4"/>
-      <c r="AI21" s="4"/>
-      <c r="AJ21" s="4"/>
-      <c r="AK21" s="4"/>
-      <c r="AL21" s="4"/>
-      <c r="AM21" s="4"/>
-      <c r="AN21" s="4"/>
-      <c r="AO21" s="4"/>
-      <c r="AP21" s="4"/>
-      <c r="AQ21" s="4"/>
-      <c r="AR21" s="4"/>
-      <c r="AS21" s="4"/>
-      <c r="AT21" s="4"/>
-      <c r="AU21" s="4"/>
-      <c r="AV21" s="4"/>
-      <c r="AW21" s="4"/>
-      <c r="AX21" s="4"/>
-      <c r="AY21" s="4"/>
-      <c r="AZ21" s="4"/>
-      <c r="BA21" s="4"/>
-      <c r="BB21" s="4"/>
-      <c r="BC21" s="4"/>
-      <c r="BD21" s="4"/>
-      <c r="BE21" s="4"/>
+      <c r="C21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="4">
+        <f>COUNT(D4:D20)</f>
+        <v>15</v>
+      </c>
+      <c r="E21" s="4">
+        <f t="shared" ref="E21:BE21" si="0">COUNT(E4:E20)</f>
+        <v>11</v>
+      </c>
+      <c r="F21" s="4">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="G21" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H21" s="4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="I21" s="4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="J21" s="4">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="K21" s="4">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="L21" s="4">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="M21" s="4">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="N21" s="4">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="O21" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="P21" s="4">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="Q21" s="4">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="R21" s="4">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="S21" s="4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="T21" s="4">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="U21" s="4">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="V21" s="4">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="W21" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="X21" s="4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="Y21" s="4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="Z21" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="AA21" s="4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="AB21" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="AC21" s="4">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="AD21" s="4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="AE21" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="AF21" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="AG21" s="4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="AH21" s="4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="AI21" s="4">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="AJ21" s="4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="AK21" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="AL21" s="4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="AM21" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="AN21" s="4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="AO21" s="4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="AP21" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="AQ21" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="AR21" s="4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="AS21" s="4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="AT21" s="4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="AU21" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="AV21" s="4">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="AW21" s="4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="AX21" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="AY21" s="4">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="AZ21" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="BA21" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="BB21" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="BC21" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="BD21" s="4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="BE21" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="BF21" s="4"/>
       <c r="BG21" s="4"/>
       <c r="BH21" s="4"/>
@@ -11263,6 +12764,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -11271,7 +12773,7 @@
   <dimension ref="A1:AC152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+      <selection activeCell="AB15" sqref="AA15:AB15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12913,4 +14415,235 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="D6:E33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="6" spans="4:5">
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="4:5" ht="15.75" thickBot="1"/>
+    <row r="8" spans="4:5" ht="15.75" thickBot="1">
+      <c r="D8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="8">
+        <v>8.1670000000000006E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="4:5" ht="15.75" thickBot="1">
+      <c r="D9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="8">
+        <v>1.4919999999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="4:5" ht="15.75" thickBot="1">
+      <c r="D10" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="8">
+        <v>2.7820000000000001E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="4:5" ht="15.75" thickBot="1">
+      <c r="D11" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="8">
+        <v>4.2529999999999998E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="4:5" ht="15.75" thickBot="1">
+      <c r="D12" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0.12701999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="4:5" ht="15.75" thickBot="1">
+      <c r="D13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="8">
+        <v>2.2280000000000001E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="4:5" ht="15.75" thickBot="1">
+      <c r="D14" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="8">
+        <v>2.0150000000000001E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="4:5" ht="15.75" thickBot="1">
+      <c r="D15" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="8">
+        <v>6.0940000000000001E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="4:5" ht="15.75" thickBot="1">
+      <c r="D16" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="8">
+        <v>6.966E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" ht="15.75" thickBot="1">
+      <c r="D17" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="8">
+        <v>1.5299999999999999E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5" ht="15.75" thickBot="1">
+      <c r="D18" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="8">
+        <v>7.7200000000000003E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5" ht="15.75" thickBot="1">
+      <c r="D19" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="8">
+        <v>4.0250000000000001E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5" ht="15.75" thickBot="1">
+      <c r="D20" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="8">
+        <v>2.4060000000000002E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="4:5" ht="15.75" thickBot="1">
+      <c r="D21" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="8">
+        <v>6.7489999999999994E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="4:5" ht="15.75" thickBot="1">
+      <c r="D22" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="8">
+        <v>7.5069999999999998E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="4:5" ht="15.75" thickBot="1">
+      <c r="D23" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="8">
+        <v>1.9290000000000002E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="4:5" ht="15.75" thickBot="1">
+      <c r="D24" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="8">
+        <v>9.5E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="4:5" ht="15.75" thickBot="1">
+      <c r="D25" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" s="8">
+        <v>5.987E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="4:5" ht="15.75" thickBot="1">
+      <c r="D26" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26" s="8">
+        <v>6.3270000000000007E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="4:5" ht="15.75" thickBot="1">
+      <c r="D27" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" s="8">
+        <v>9.0560000000000002E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="4:5" ht="15.75" thickBot="1">
+      <c r="D28" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="8">
+        <v>2.758E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="4:5" ht="15.75" thickBot="1">
+      <c r="D29" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="8">
+        <v>9.7800000000000005E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="4:5" ht="15.75" thickBot="1">
+      <c r="D30" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="8">
+        <v>2.3599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="4:5" ht="15.75" thickBot="1">
+      <c r="D31" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E31" s="8">
+        <v>1.5E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="4:5" ht="15.75" thickBot="1">
+      <c r="D32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" s="8">
+        <v>1.9740000000000001E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5" ht="15.75" thickBot="1">
+      <c r="D33" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" s="8">
+        <v>7.3999999999999999E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Report Development, altered results
added design to report, altered results following bugfix
</commit_message>
<xml_diff>
--- a/Documentation/Design/Cipher Models.xlsx
+++ b/Documentation/Design/Cipher Models.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="29">
   <si>
     <t>Character Frequency</t>
   </si>
@@ -110,7 +110,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,8 +145,14 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF494949"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -159,8 +165,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -192,11 +204,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFE0E0E0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -216,6 +237,15 @@
     <xf numFmtId="10" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,24 +502,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="67988096"/>
-        <c:axId val="68005248"/>
+        <c:axId val="88964096"/>
+        <c:axId val="94855168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="67988096"/>
+        <c:axId val="88964096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68005248"/>
+        <c:crossAx val="94855168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68005248"/>
+        <c:axId val="94855168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="24"/>
@@ -498,7 +528,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67988096"/>
+        <c:crossAx val="88964096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="2"/>
@@ -508,7 +538,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -726,17 +756,17 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="82427264"/>
-        <c:axId val="82441344"/>
+        <c:axId val="97390592"/>
+        <c:axId val="97392128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="82427264"/>
+        <c:axId val="97390592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82441344"/>
+        <c:crossAx val="97392128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -744,7 +774,7 @@
         <c:tickLblSkip val="2"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82441344"/>
+        <c:axId val="97392128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -752,7 +782,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82427264"/>
+        <c:crossAx val="97390592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -761,7 +791,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -772,7 +802,14 @@
   <c:lang val="en-GB"/>
   <c:chart>
     <c:title>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13619444444444448"/>
+          <c:y val="2.6755852842809371E-2"/>
+        </c:manualLayout>
+      </c:layout>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -967,24 +1004,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="74192768"/>
-        <c:axId val="74194304"/>
+        <c:axId val="97645696"/>
+        <c:axId val="97647232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="74192768"/>
+        <c:axId val="97645696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74194304"/>
+        <c:crossAx val="97647232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74194304"/>
+        <c:axId val="97647232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -992,7 +1029,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74192768"/>
+        <c:crossAx val="97645696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1001,7 +1038,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1081,16 +1118,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -14419,226 +14456,1116 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="D6:E33"/>
+  <dimension ref="D6:V34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="6" spans="4:5">
+    <row r="6" spans="4:22" ht="16.5" thickBot="1">
       <c r="E6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="4:5" ht="15.75" thickBot="1"/>
-    <row r="8" spans="4:5" ht="15.75" thickBot="1">
+      <c r="Q6" s="9"/>
+      <c r="R6" s="10"/>
+      <c r="U6" t="s">
+        <v>6</v>
+      </c>
+      <c r="V6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="4:22" ht="16.5" thickBot="1">
+      <c r="K7">
+        <f>SUM(54/100)</f>
+        <v>0.54</v>
+      </c>
+      <c r="N7">
+        <v>0.63</v>
+      </c>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="10"/>
+      <c r="U7" t="s">
+        <v>21</v>
+      </c>
+      <c r="V7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="4:22" ht="16.5" thickBot="1">
       <c r="D8" s="7" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="8">
         <v>8.1670000000000006E-2</v>
       </c>
-    </row>
-    <row r="9" spans="4:5" ht="15.75" thickBot="1">
+      <c r="F8" s="13">
+        <f>ROUND(E8,2)</f>
+        <v>0.08</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>8</v>
+      </c>
+      <c r="K8">
+        <f>SUM($K$7*H8)</f>
+        <v>4.32</v>
+      </c>
+      <c r="L8">
+        <f>ROUND(K8,0)</f>
+        <v>4</v>
+      </c>
+      <c r="N8">
+        <f>SUM($N$7*H8)</f>
+        <v>5.04</v>
+      </c>
+      <c r="O8">
+        <f>ROUND(N8,0)</f>
+        <v>5</v>
+      </c>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="10"/>
+      <c r="U8" t="s">
+        <v>2</v>
+      </c>
+      <c r="V8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="4:22" ht="16.5" thickBot="1">
       <c r="D9" s="7" t="s">
         <v>3</v>
       </c>
       <c r="E9" s="8">
         <v>1.4919999999999999E-2</v>
       </c>
-    </row>
-    <row r="10" spans="4:5" ht="15.75" thickBot="1">
+      <c r="F9" s="12">
+        <f>ROUND(E9,2)</f>
+        <v>0.01</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <f>SUM($K$7*H9)</f>
+        <v>0.54</v>
+      </c>
+      <c r="L9">
+        <f t="shared" ref="L9:L33" si="0">ROUND(K9,0)</f>
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <f t="shared" ref="N9:N33" si="1">SUM($N$7*H9)</f>
+        <v>0.63</v>
+      </c>
+      <c r="O9">
+        <f t="shared" ref="O9:O33" si="2">ROUND(N9,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="10"/>
+      <c r="U9" t="s">
+        <v>10</v>
+      </c>
+      <c r="V9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="4:22" ht="16.5" thickBot="1">
       <c r="D10" s="7" t="s">
         <v>4</v>
       </c>
       <c r="E10" s="8">
         <v>2.7820000000000001E-2</v>
       </c>
-    </row>
-    <row r="11" spans="4:5" ht="15.75" thickBot="1">
+      <c r="F10" s="12">
+        <f t="shared" ref="F10:F33" si="3">ROUND(E10,2)</f>
+        <v>0.03</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+      <c r="K10">
+        <f t="shared" ref="K10:K33" si="4">SUM($K$7*H10)</f>
+        <v>1.62</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="1"/>
+        <v>1.8900000000000001</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="10"/>
+      <c r="U10" t="s">
+        <v>15</v>
+      </c>
+      <c r="V10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="4:22" ht="16.5" thickBot="1">
       <c r="D11" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="8">
         <v>4.2529999999999998E-2</v>
       </c>
-    </row>
-    <row r="12" spans="4:5" ht="15.75" thickBot="1">
+      <c r="F11" s="12">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="4"/>
+        <v>2.16</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="1"/>
+        <v>2.52</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="10"/>
+      <c r="U11" t="s">
+        <v>16</v>
+      </c>
+      <c r="V11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="4:22" ht="16.5" thickBot="1">
       <c r="D12" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E12" s="8">
         <v>0.12701999999999999</v>
       </c>
-    </row>
-    <row r="13" spans="4:5" ht="15.75" thickBot="1">
+      <c r="F12" s="12">
+        <f t="shared" si="3"/>
+        <v>0.13</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12">
+        <v>13</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="4"/>
+        <v>7.0200000000000005</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="1"/>
+        <v>8.19</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="10"/>
+      <c r="U12" t="s">
+        <v>20</v>
+      </c>
+      <c r="V12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="4:22" ht="16.5" thickBot="1">
       <c r="D13" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="8">
         <v>2.2280000000000001E-2</v>
       </c>
-    </row>
-    <row r="14" spans="4:5" ht="15.75" thickBot="1">
+      <c r="F13" s="12">
+        <f t="shared" si="3"/>
+        <v>0.02</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="4"/>
+        <v>1.08</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="1"/>
+        <v>1.26</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="10"/>
+      <c r="U13" t="s">
+        <v>9</v>
+      </c>
+      <c r="V13">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="14" spans="4:22" ht="16.5" thickBot="1">
       <c r="D14" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E14" s="8">
         <v>2.0150000000000001E-2</v>
       </c>
-    </row>
-    <row r="15" spans="4:5" ht="15.75" thickBot="1">
+      <c r="F14" s="12">
+        <f t="shared" si="3"/>
+        <v>0.02</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="4"/>
+        <v>1.08</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="1"/>
+        <v>1.26</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="10"/>
+      <c r="U14" t="s">
+        <v>19</v>
+      </c>
+      <c r="V14">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="15" spans="4:22" ht="16.5" thickBot="1">
       <c r="D15" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="8">
         <v>6.0940000000000001E-2</v>
       </c>
-    </row>
-    <row r="16" spans="4:5" ht="15.75" thickBot="1">
+      <c r="F15" s="12">
+        <f t="shared" si="3"/>
+        <v>0.06</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15">
+        <v>6</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="4"/>
+        <v>3.24</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="1"/>
+        <v>3.7800000000000002</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="10"/>
+      <c r="U15" t="s">
+        <v>5</v>
+      </c>
+      <c r="V15">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="4:22" ht="16.5" thickBot="1">
       <c r="D16" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E16" s="8">
         <v>6.966E-2</v>
       </c>
-    </row>
-    <row r="17" spans="4:5" ht="15.75" thickBot="1">
+      <c r="F16" s="12">
+        <f t="shared" si="3"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16">
+        <v>7</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="4"/>
+        <v>3.7800000000000002</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="1"/>
+        <v>4.41</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="10"/>
+      <c r="U16" t="s">
+        <v>13</v>
+      </c>
+      <c r="V16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="4:22" ht="16.5" thickBot="1">
       <c r="D17" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E17" s="8">
         <v>1.5299999999999999E-3</v>
       </c>
-    </row>
-    <row r="18" spans="4:5" ht="15.75" thickBot="1">
+      <c r="F17" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="10"/>
+      <c r="U17" t="s">
+        <v>22</v>
+      </c>
+      <c r="V17">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="18" spans="4:22" ht="16.5" thickBot="1">
       <c r="D18" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E18" s="8">
         <v>7.7200000000000003E-3</v>
       </c>
-    </row>
-    <row r="19" spans="4:5" ht="15.75" thickBot="1">
+      <c r="F18" s="12">
+        <f t="shared" si="3"/>
+        <v>0.01</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="4"/>
+        <v>0.54</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="1"/>
+        <v>0.63</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="10"/>
+      <c r="U18" t="s">
+        <v>4</v>
+      </c>
+      <c r="V18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="4:22" ht="16.5" thickBot="1">
       <c r="D19" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E19" s="8">
         <v>4.0250000000000001E-2</v>
       </c>
-    </row>
-    <row r="20" spans="4:5" ht="15.75" thickBot="1">
+      <c r="F19" s="12">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19">
+        <v>4</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="4"/>
+        <v>2.16</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="1"/>
+        <v>2.52</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="10"/>
+      <c r="U19" t="s">
+        <v>14</v>
+      </c>
+      <c r="V19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="4:22" ht="16.5" thickBot="1">
       <c r="D20" s="7" t="s">
         <v>14</v>
       </c>
       <c r="E20" s="8">
         <v>2.4060000000000002E-2</v>
       </c>
-    </row>
-    <row r="21" spans="4:5" ht="15.75" thickBot="1">
+      <c r="F20" s="12">
+        <f t="shared" si="3"/>
+        <v>0.02</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="4"/>
+        <v>1.08</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="1"/>
+        <v>1.26</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="U20" t="s">
+        <v>7</v>
+      </c>
+      <c r="V20">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="21" spans="4:22" ht="16.5" thickBot="1">
       <c r="D21" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E21" s="8">
         <v>6.7489999999999994E-2</v>
       </c>
-    </row>
-    <row r="22" spans="4:5" ht="15.75" thickBot="1">
+      <c r="F21" s="12">
+        <f t="shared" si="3"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21">
+        <v>7</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="4"/>
+        <v>3.7800000000000002</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="1"/>
+        <v>4.41</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="U21" t="s">
+        <v>24</v>
+      </c>
+      <c r="V21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="4:22" ht="16.5" thickBot="1">
       <c r="D22" s="7" t="s">
         <v>16</v>
       </c>
       <c r="E22" s="8">
         <v>7.5069999999999998E-2</v>
       </c>
-    </row>
-    <row r="23" spans="4:5" ht="15.75" thickBot="1">
+      <c r="F22" s="12">
+        <f t="shared" si="3"/>
+        <v>0.08</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22">
+        <v>8</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="4"/>
+        <v>4.32</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="1"/>
+        <v>5.04</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="U22" t="s">
+        <v>26</v>
+      </c>
+      <c r="V22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="4:22" ht="16.5" thickBot="1">
       <c r="D23" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E23" s="8">
         <v>1.9290000000000002E-2</v>
       </c>
-    </row>
-    <row r="24" spans="4:5" ht="15.75" thickBot="1">
+      <c r="F23" s="12">
+        <f t="shared" si="3"/>
+        <v>0.02</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="4"/>
+        <v>1.08</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="1"/>
+        <v>1.26</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
+      <c r="U23" t="s">
+        <v>8</v>
+      </c>
+      <c r="V23">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="24" spans="4:22" ht="15.75" thickBot="1">
       <c r="D24" s="7" t="s">
         <v>18</v>
       </c>
       <c r="E24" s="8">
         <v>9.5E-4</v>
       </c>
-    </row>
-    <row r="25" spans="4:5" ht="15.75" thickBot="1">
+      <c r="F24" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U24" t="s">
+        <v>17</v>
+      </c>
+      <c r="V24">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="25" spans="4:22" ht="15.75" thickBot="1">
       <c r="D25" s="7" t="s">
         <v>19</v>
       </c>
       <c r="E25" s="8">
         <v>5.987E-2</v>
       </c>
-    </row>
-    <row r="26" spans="4:5" ht="15.75" thickBot="1">
+      <c r="F25" s="12">
+        <f t="shared" si="3"/>
+        <v>0.06</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H25">
+        <v>6</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="4"/>
+        <v>3.24</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="1"/>
+        <v>3.7800000000000002</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="U25" t="s">
+        <v>3</v>
+      </c>
+      <c r="V25">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="26" spans="4:22" ht="15.75" thickBot="1">
       <c r="D26" s="7" t="s">
         <v>20</v>
       </c>
       <c r="E26" s="8">
         <v>6.3270000000000007E-2</v>
       </c>
-    </row>
-    <row r="27" spans="4:5" ht="15.75" thickBot="1">
+      <c r="F26" s="12">
+        <f t="shared" si="3"/>
+        <v>0.06</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26">
+        <v>6</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="4"/>
+        <v>3.24</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="1"/>
+        <v>3.7800000000000002</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="U26" t="s">
+        <v>23</v>
+      </c>
+      <c r="V26">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="27" spans="4:22" ht="15.75" thickBot="1">
       <c r="D27" s="7" t="s">
         <v>21</v>
       </c>
       <c r="E27" s="8">
         <v>9.0560000000000002E-2</v>
       </c>
-    </row>
-    <row r="28" spans="4:5" ht="15.75" thickBot="1">
+      <c r="F27" s="12">
+        <f t="shared" si="3"/>
+        <v>0.09</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H27">
+        <v>9</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="4"/>
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="1"/>
+        <v>5.67</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="U27" t="s">
+        <v>12</v>
+      </c>
+      <c r="V27">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="28" spans="4:22" ht="15.75" thickBot="1">
       <c r="D28" s="7" t="s">
         <v>22</v>
       </c>
       <c r="E28" s="8">
         <v>2.758E-2</v>
       </c>
-    </row>
-    <row r="29" spans="4:5" ht="15.75" thickBot="1">
+      <c r="F28" s="12">
+        <f t="shared" si="3"/>
+        <v>0.03</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H28">
+        <v>3</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="4"/>
+        <v>1.62</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="1"/>
+        <v>1.8900000000000001</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="U28" t="s">
+        <v>18</v>
+      </c>
+      <c r="V28">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="29" spans="4:22" ht="15.75" thickBot="1">
       <c r="D29" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E29" s="8">
         <v>9.7800000000000005E-3</v>
       </c>
-    </row>
-    <row r="30" spans="4:5" ht="15.75" thickBot="1">
+      <c r="F29" s="12">
+        <f t="shared" si="3"/>
+        <v>0.01</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="4"/>
+        <v>0.54</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="1"/>
+        <v>0.63</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="U29" t="s">
+        <v>11</v>
+      </c>
+      <c r="V29">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="30" spans="4:22" ht="15.75" thickBot="1">
       <c r="D30" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E30" s="8">
         <v>2.3599999999999999E-2</v>
       </c>
-    </row>
-    <row r="31" spans="4:5" ht="15.75" thickBot="1">
+      <c r="F30" s="12">
+        <f t="shared" si="3"/>
+        <v>0.02</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H30">
+        <v>2</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="4"/>
+        <v>1.08</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="1"/>
+        <v>1.26</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="U30" t="s">
+        <v>25</v>
+      </c>
+      <c r="V30">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="31" spans="4:22" ht="15.75" thickBot="1">
       <c r="D31" s="7" t="s">
         <v>25</v>
       </c>
       <c r="E31" s="8">
         <v>1.5E-3</v>
       </c>
-    </row>
-    <row r="32" spans="4:5" ht="15.75" thickBot="1">
+      <c r="F31" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U31" t="s">
+        <v>27</v>
+      </c>
+      <c r="V31">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="32" spans="4:22" ht="15.75" thickBot="1">
       <c r="D32" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E32" s="8">
         <v>1.9740000000000001E-2</v>
       </c>
-    </row>
-    <row r="33" spans="4:5" ht="15.75" thickBot="1">
+      <c r="F32" s="12">
+        <f t="shared" si="3"/>
+        <v>0.02</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H32">
+        <v>2</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="4"/>
+        <v>1.08</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="1"/>
+        <v>1.26</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="4:15" ht="15.75" thickBot="1">
       <c r="D33" s="7" t="s">
         <v>27</v>
       </c>
       <c r="E33" s="8">
         <v>7.3999999999999999E-4</v>
+      </c>
+      <c r="F33" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="4:15">
+      <c r="F34" s="11">
+        <f>SUM(F8:F33)</f>
+        <v>0.9900000000000001</v>
+      </c>
+      <c r="L34">
+        <f>SUM(L8:L33)</f>
+        <v>54</v>
+      </c>
+      <c r="O34">
+        <f>SUM(O8:O33)</f>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>